<commit_message>
Added new functions for future teacher login and register
- Added set_pwhash in models.py
- Added check_password in models.py
- Added new columns for Teacher: validated (bool), phone (string), email (string), pwhash (string)
- Teacher.validated will be used for admins to validate a newly registered teacher.
- Imported libraries for login management and password managements
</commit_message>
<xml_diff>
--- a/API List.xlsx
+++ b/API List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DJ\Desktop\flaskAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA1B57B-5E9B-41FB-A3E6-9782AB250288}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475E1F0A-5351-49CA-9FB9-AB71B58CDAAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -536,12 +536,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -824,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,1199 +840,1199 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3" t="s">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3" t="s">
+      <c r="E13" s="2"/>
+      <c r="F13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="3"/>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="3"/>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3" t="s">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3" t="s">
+      <c r="D21" s="2"/>
+      <c r="E21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G21" s="3"/>
+      <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3" t="s">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G22" s="3"/>
+      <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3" t="s">
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="3"/>
+      <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G24" s="3"/>
+      <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3" t="s">
+      <c r="E25" s="2"/>
+      <c r="F25" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3" t="s">
+      <c r="D30" s="2"/>
+      <c r="E30" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G30" s="3"/>
+      <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3" t="s">
+      <c r="E31" s="2"/>
+      <c r="F31" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G31" s="3"/>
+      <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3" t="s">
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G32" s="3"/>
+      <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G33" s="3"/>
+      <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3" t="s">
+      <c r="E34" s="2"/>
+      <c r="F34" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G34" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E38" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G38" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3" t="s">
+      <c r="D39" s="2"/>
+      <c r="E39" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F39" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G39" s="3"/>
+      <c r="G39" s="2"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3" t="s">
+      <c r="D40" s="2"/>
+      <c r="E40" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F40" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G40" s="3"/>
+      <c r="G40" s="2"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3" t="s">
+      <c r="E41" s="2"/>
+      <c r="F41" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G41" s="3"/>
+      <c r="G41" s="2"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3" t="s">
+      <c r="E42" s="2"/>
+      <c r="F42" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G42" s="3"/>
+      <c r="G42" s="2"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3" t="s">
+      <c r="E43" s="2"/>
+      <c r="F43" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="G43" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E47" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F47" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="G47" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3" t="s">
+      <c r="D48" s="2"/>
+      <c r="E48" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="F48" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G48" s="3"/>
+      <c r="G48" s="2"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3" t="s">
+      <c r="D49" s="2"/>
+      <c r="E49" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="F49" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G49" s="3"/>
+      <c r="G49" s="2"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3" t="s">
+      <c r="E50" s="2"/>
+      <c r="F50" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G50" s="3"/>
+      <c r="G50" s="2"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3" t="s">
+      <c r="E51" s="2"/>
+      <c r="F51" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G51" s="3"/>
+      <c r="G51" s="2"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3" t="s">
+      <c r="E52" s="2"/>
+      <c r="F52" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="G52" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D56" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="E56" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="F56" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G56" s="2" t="s">
+      <c r="G56" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3" t="s">
+      <c r="D57" s="2"/>
+      <c r="E57" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="F57" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G57" s="3"/>
+      <c r="G57" s="2"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3" t="s">
+      <c r="D58" s="2"/>
+      <c r="E58" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F58" s="3" t="s">
+      <c r="F58" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G58" s="3"/>
+      <c r="G58" s="2"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3" t="s">
+      <c r="E59" s="2"/>
+      <c r="F59" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G59" s="3"/>
+      <c r="G59" s="2"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3" t="s">
+      <c r="E60" s="2"/>
+      <c r="F60" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="G60" s="3"/>
+      <c r="G60" s="2"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B61" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D61" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3" t="s">
+      <c r="E61" s="2"/>
+      <c r="F61" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="G61" s="3" t="s">
+      <c r="G61" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+      <c r="A65" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D65" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="E65" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F65" s="2" t="s">
+      <c r="F65" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G65" s="2" t="s">
+      <c r="G65" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C66" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3" t="s">
+      <c r="D66" s="2"/>
+      <c r="E66" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F66" s="3" t="s">
+      <c r="F66" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="G66" s="3"/>
+      <c r="G66" s="2"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B67" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C67" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3" t="s">
+      <c r="D67" s="2"/>
+      <c r="E67" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F67" s="3" t="s">
+      <c r="F67" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="G67" s="3"/>
+      <c r="G67" s="2"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C68" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D68" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3" t="s">
+      <c r="E68" s="2"/>
+      <c r="F68" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="G68" s="3"/>
+      <c r="G68" s="2"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C69" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D69" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3" t="s">
+      <c r="E69" s="2"/>
+      <c r="F69" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G69" s="3"/>
+      <c r="G69" s="2"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
+      <c r="A70" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C70" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D70" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3" t="s">
+      <c r="E70" s="2"/>
+      <c r="F70" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G70" s="3" t="s">
+      <c r="G70" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="4"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+      <c r="A74" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B74" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C74" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D74" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="E74" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="F74" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G74" s="2" t="s">
+      <c r="G74" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C75" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3" t="s">
+      <c r="D75" s="2"/>
+      <c r="E75" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F75" s="3" t="s">
+      <c r="F75" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="G75" s="3"/>
+      <c r="G75" s="2"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="C76" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3" t="s">
+      <c r="D76" s="2"/>
+      <c r="E76" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F76" s="3" t="s">
+      <c r="F76" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="G76" s="3"/>
+      <c r="G76" s="2"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="C77" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D77" s="3" t="s">
+      <c r="D77" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3" t="s">
+      <c r="E77" s="2"/>
+      <c r="F77" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="G77" s="3"/>
+      <c r="G77" s="2"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+      <c r="A78" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="C78" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D78" s="3" t="s">
+      <c r="D78" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3" t="s">
+      <c r="E78" s="2"/>
+      <c r="F78" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="G78" s="3"/>
+      <c r="G78" s="2"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="C79" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D79" s="3" t="s">
+      <c r="D79" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3" t="s">
+      <c r="E79" s="2"/>
+      <c r="F79" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="G79" s="3" t="s">
+      <c r="G79" s="2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2073,133 +2073,133 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Combined user and teacher and realized some apis, but need to work on unified entry point for all db operation
</commit_message>
<xml_diff>
--- a/API List.xlsx
+++ b/API List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DJ\Desktop\flaskAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95C462B-6F17-467B-8C74-FB5348247700}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE84CEE-2722-4C59-B330-8D9A04F56F70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="188">
   <si>
     <t>API Name</t>
   </si>
@@ -505,9 +505,6 @@
     <t>student_id, name</t>
   </si>
   <si>
-    <t>teacher_id, principle_id</t>
-  </si>
-  <si>
     <t>Approve a registerd teacher</t>
   </si>
   <si>
@@ -529,9 +526,6 @@
     <t>Authorization</t>
   </si>
   <si>
-    <t>login_teacher</t>
-  </si>
-  <si>
     <t>/api/v1.0/auth/login</t>
   </si>
   <si>
@@ -565,9 +559,6 @@
     <t>Revoke all tokens associated with the access_token bearer</t>
   </si>
   <si>
-    <t>wechat_login</t>
-  </si>
-  <si>
     <t>/api/v1.0/wechat/login</t>
   </si>
   <si>
@@ -602,6 +593,12 @@
   </si>
   <si>
     <t>Headers</t>
+  </si>
+  <si>
+    <t>login_web</t>
+  </si>
+  <si>
+    <t>login_wechat</t>
   </si>
 </sst>
 </file>
@@ -1011,7 +1008,7 @@
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1042,7 +1039,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1057,10 +1054,10 @@
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>2</v>
@@ -1070,7 +1067,9 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" s="8"/>
+      <c r="A3" s="8" t="s">
+        <v>160</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1085,7 +1084,7 @@
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>22</v>
@@ -1219,7 +1218,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>0</v>
@@ -1234,10 +1233,10 @@
         <v>7</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>2</v>
@@ -1248,7 +1247,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>28</v>
@@ -1262,13 +1261,13 @@
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
@@ -1371,12 +1370,14 @@
       <c r="E17" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>172</v>
+      </c>
       <c r="G17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>156</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>157</v>
       </c>
       <c r="I17" s="2"/>
     </row>
@@ -1405,7 +1406,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>0</v>
@@ -1420,10 +1421,10 @@
         <v>7</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>2</v>
@@ -1434,7 +1435,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>41</v>
@@ -1443,7 +1444,7 @@
         <v>42</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>8</v>
@@ -1558,7 +1559,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>0</v>
@@ -1571,10 +1572,10 @@
         <v>7</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>2</v>
@@ -1705,7 +1706,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>0</v>
@@ -1718,10 +1719,10 @@
         <v>7</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>2</v>
@@ -1852,7 +1853,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>0</v>
@@ -1865,10 +1866,10 @@
         <v>7</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>2</v>
@@ -1999,7 +2000,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>0</v>
@@ -2012,10 +2013,10 @@
         <v>7</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>2</v>
@@ -2146,7 +2147,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>0</v>
@@ -2159,10 +2160,10 @@
         <v>7</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>2</v>
@@ -2293,7 +2294,7 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>0</v>
@@ -2306,10 +2307,10 @@
         <v>7</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>2</v>
@@ -2428,7 +2429,7 @@
     <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A84" s="8"/>
       <c r="B84" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C84" s="10"/>
       <c r="D84" s="10"/>
@@ -2440,7 +2441,7 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A85" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>0</v>
@@ -2453,10 +2454,10 @@
         <v>7</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>2</v>
@@ -2467,13 +2468,13 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A86" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="2" t="s">
@@ -2481,68 +2482,68 @@
       </c>
       <c r="F86" s="2"/>
       <c r="G86" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I86" s="2"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A87" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D87" s="2"/>
       <c r="E87" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G87" s="2"/>
       <c r="H87" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I87" s="2"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A88" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G88" s="2"/>
       <c r="H88" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I88" s="2"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A89" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D89" s="2"/>
       <c r="E89" s="2" t="s">
@@ -2550,10 +2551,10 @@
       </c>
       <c r="F89" s="2"/>
       <c r="G89" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I89" s="2"/>
     </row>
@@ -2593,7 +2594,7 @@
     <row r="95" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A95" s="8"/>
       <c r="B95" s="10" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C95" s="10"/>
       <c r="D95" s="10"/>
@@ -2605,7 +2606,7 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A96" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>0</v>
@@ -2620,10 +2621,10 @@
         <v>7</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>2</v>
@@ -2635,13 +2636,13 @@
     <row r="97" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A97" s="8"/>
       <c r="B97" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>8</v>
@@ -2651,7 +2652,7 @@
         <v>31</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I97" s="2"/>
     </row>
@@ -2701,17 +2702,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B48:I48"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B30:I30"/>
+    <mergeCell ref="B39:I39"/>
     <mergeCell ref="B95:I95"/>
     <mergeCell ref="B84:I84"/>
     <mergeCell ref="B57:I57"/>
     <mergeCell ref="B66:I66"/>
     <mergeCell ref="B75:I75"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="B30:I30"/>
-    <mergeCell ref="B39:I39"/>
-    <mergeCell ref="B48:I48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Realized add real information for teacher
</commit_message>
<xml_diff>
--- a/API List.xlsx
+++ b/API List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DJ\Desktop\flaskAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B542F7-89F8-471C-A3D2-4179C5D0C28A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC35E64B-8A7F-4406-8CEB-7512195ED096}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23970" yWindow="9270" windowWidth="28800" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="2805" windowWidth="28800" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="189">
   <si>
     <t>API Name</t>
   </si>
@@ -556,12 +556,6 @@
     <t>Login using wechat</t>
   </si>
   <si>
-    <t>Register a new teacher</t>
-  </si>
-  <si>
-    <t>realName, phone, email, password</t>
-  </si>
-  <si>
     <t>Needs approvement</t>
   </si>
   <si>
@@ -599,6 +593,15 @@
   </si>
   <si>
     <t>Update or create a parent_hood's information</t>
+  </si>
+  <si>
+    <t>everybody</t>
+  </si>
+  <si>
+    <t>realName, phone</t>
+  </si>
+  <si>
+    <t>Fill in real information of a teacher from wechat</t>
   </si>
 </sst>
 </file>
@@ -1008,7 +1011,7 @@
   <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,8 +1022,8 @@
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" customWidth="1"/>
-    <col min="8" max="8" width="28.42578125" customWidth="1"/>
+    <col min="7" max="7" width="36.140625" customWidth="1"/>
+    <col min="8" max="8" width="47.5703125" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1054,7 +1057,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>155</v>
@@ -1233,7 +1236,7 @@
         <v>7</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>155</v>
@@ -1255,19 +1258,21 @@
       <c r="C12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>186</v>
+      </c>
       <c r="E12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="H12" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1423,7 +1428,7 @@
         <v>7</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>155</v>
@@ -1574,7 +1579,7 @@
         <v>7</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>155</v>
@@ -1721,7 +1726,7 @@
         <v>7</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>155</v>
@@ -1870,7 +1875,7 @@
         <v>7</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>155</v>
@@ -1898,10 +1903,10 @@
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I50" s="2"/>
     </row>
@@ -2000,7 +2005,7 @@
         <v>7</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>155</v>
@@ -2023,14 +2028,14 @@
         <v>99</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H58" s="2" t="s">
         <v>101</v>
@@ -2151,7 +2156,7 @@
         <v>7</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>155</v>
@@ -2298,7 +2303,7 @@
         <v>7</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>155</v>
@@ -2445,7 +2450,7 @@
         <v>7</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>155</v>
@@ -2462,7 +2467,7 @@
         <v>156</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>159</v>
@@ -2531,7 +2536,7 @@
         <v>156</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>170</v>
@@ -2585,7 +2590,7 @@
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="8"/>
       <c r="B94" s="10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C94" s="10"/>
       <c r="D94" s="10"/>
@@ -2612,7 +2617,7 @@
         <v>7</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>155</v>
@@ -2627,13 +2632,13 @@
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="8"/>
       <c r="B96" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D96" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>8</v>
@@ -2643,7 +2648,7 @@
         <v>31</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I96" s="2"/>
     </row>
@@ -2693,17 +2698,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B94:I94"/>
+    <mergeCell ref="B83:I83"/>
+    <mergeCell ref="B56:I56"/>
+    <mergeCell ref="B65:I65"/>
+    <mergeCell ref="B74:I74"/>
     <mergeCell ref="B48:I48"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B21:I21"/>
     <mergeCell ref="B30:I30"/>
     <mergeCell ref="B39:I39"/>
-    <mergeCell ref="B94:I94"/>
-    <mergeCell ref="B83:I83"/>
-    <mergeCell ref="B56:I56"/>
-    <mergeCell ref="B65:I65"/>
-    <mergeCell ref="B74:I74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Working on add class session and get a list of course credits for a student APIs
</commit_message>
<xml_diff>
--- a/API List.xlsx
+++ b/API List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DJ\Desktop\flaskAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2665C7D8-453C-4828-80EF-3AB9AC7EC758}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50426CD5-70E1-4E36-8C6A-6D56A7F630BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23820" yWindow="6750" windowWidth="28800" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21075" yWindow="3165" windowWidth="28800" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="189">
   <si>
     <t>API Name</t>
   </si>
@@ -1010,15 +1010,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" customWidth="1"/>
@@ -1721,7 +1721,9 @@
       <c r="C40" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D40" s="1"/>
+      <c r="D40" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="E40" s="1" t="s">
         <v>7</v>
       </c>
@@ -1790,14 +1792,16 @@
       <c r="C43" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D43" s="2"/>
+      <c r="D43" s="2" t="s">
+        <v>182</v>
+      </c>
       <c r="E43" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F43" s="2"/>
+      <c r="G43" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G43" s="2"/>
       <c r="H43" s="2" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
Scheduling recurring class sessions realized
</commit_message>
<xml_diff>
--- a/API List.xlsx
+++ b/API List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DJ\Desktop\flaskAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50426CD5-70E1-4E36-8C6A-6D56A7F630BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA23B5C-0AAA-4A14-AE6B-E2EFFF196B53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21075" yWindow="3165" windowWidth="28800" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="833" yWindow="-98" windowWidth="18465" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -340,9 +340,6 @@
     <t>course_id, info</t>
   </si>
   <si>
-    <t>Add one class_session</t>
-  </si>
-  <si>
     <t>update_class_session</t>
   </si>
   <si>
@@ -499,9 +496,6 @@
     <t>Implemented</t>
   </si>
   <si>
-    <t>realName, gender, DOB</t>
-  </si>
-  <si>
     <t>Body (JSON)</t>
   </si>
   <si>
@@ -601,7 +595,13 @@
     <t>Fill in real information of a teacher from wechat</t>
   </si>
   <si>
-    <t>course_id, start_time, end_time, info, repeat_weekly, repeatEndDate, [student_ids]</t>
+    <t>realName, gender, DOB (Naïve datetime, without timezone)</t>
+  </si>
+  <si>
+    <t>course_id, start_time, end_time, info, repeat_weekly, repeat_wkdays, repeat_until</t>
+  </si>
+  <si>
+    <t>Add one class_session or repeating class_sessions</t>
   </si>
 </sst>
 </file>
@@ -1010,24 +1010,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="G52" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="32.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.86328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1328125" customWidth="1"/>
+    <col min="3" max="3" width="32.265625" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="94.85546875" customWidth="1"/>
-    <col min="8" max="8" width="47.5703125" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.73046875" customWidth="1"/>
+    <col min="7" max="7" width="94.86328125" customWidth="1"/>
+    <col min="8" max="8" width="47.59765625" customWidth="1"/>
+    <col min="9" max="9" width="10.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="4"/>
       <c r="B1" s="10" t="s">
         <v>4</v>
@@ -1040,9 +1040,9 @@
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1051,16 +1051,16 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>2</v>
@@ -1069,9 +1069,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -1080,21 +1080,21 @@
         <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>154</v>
+        <v>186</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="8"/>
       <c r="B4" s="2" t="s">
         <v>10</v>
@@ -1103,7 +1103,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>11</v>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="8"/>
       <c r="B5" s="2" t="s">
         <v>14</v>
@@ -1126,7 +1126,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>11</v>
@@ -1138,7 +1138,7 @@
       </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="8"/>
       <c r="B6" s="2" t="s">
         <v>15</v>
@@ -1147,21 +1147,21 @@
         <v>13</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="8"/>
       <c r="B7" s="2" t="s">
         <v>23</v>
@@ -1170,7 +1170,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>24</v>
@@ -1186,7 +1186,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1196,7 +1196,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1206,7 +1206,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="8"/>
       <c r="B10" s="10" t="s">
         <v>27</v>
@@ -1219,9 +1219,9 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>0</v>
@@ -1230,16 +1230,16 @@
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>2</v>
@@ -1248,9 +1248,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>28</v>
@@ -1259,23 +1259,23 @@
         <v>29</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="8"/>
       <c r="B13" s="2" t="s">
         <v>30</v>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="8"/>
       <c r="B14" s="2" t="s">
         <v>33</v>
@@ -1315,7 +1315,7 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="8"/>
       <c r="B15" s="2" t="s">
         <v>36</v>
@@ -1329,14 +1329,14 @@
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>37</v>
       </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="8"/>
       <c r="B16" s="2" t="s">
         <v>38</v>
@@ -1345,7 +1345,7 @@
         <v>29</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>24</v>
@@ -1361,44 +1361,44 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B17" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>149</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>31</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="8"/>
       <c r="B21" s="11" t="s">
         <v>40</v>
@@ -1411,9 +1411,9 @@
       <c r="H21" s="12"/>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>0</v>
@@ -1422,16 +1422,16 @@
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>2</v>
@@ -1440,9 +1440,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>41</v>
@@ -1451,7 +1451,7 @@
         <v>42</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>8</v>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="8"/>
       <c r="B24" s="2" t="s">
         <v>44</v>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="8"/>
       <c r="B25" s="2" t="s">
         <v>47</v>
@@ -1505,7 +1505,7 @@
       </c>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="8"/>
       <c r="B26" s="2" t="s">
         <v>50</v>
@@ -1528,7 +1528,7 @@
       </c>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="8"/>
       <c r="B27" s="2" t="s">
         <v>52</v>
@@ -1551,7 +1551,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="8"/>
       <c r="B30" s="10" t="s">
         <v>54</v>
@@ -1564,9 +1564,9 @@
       <c r="H30" s="10"/>
       <c r="I30" s="10"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>0</v>
@@ -1579,10 +1579,10 @@
         <v>7</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>2</v>
@@ -1591,7 +1591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="8"/>
       <c r="B32" s="2" t="s">
         <v>55</v>
@@ -1612,7 +1612,7 @@
       </c>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="8"/>
       <c r="B33" s="2" t="s">
         <v>58</v>
@@ -1633,7 +1633,7 @@
       </c>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="8"/>
       <c r="B34" s="2" t="s">
         <v>61</v>
@@ -1652,7 +1652,7 @@
       </c>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="8"/>
       <c r="B35" s="2" t="s">
         <v>64</v>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="8"/>
       <c r="B36" s="2" t="s">
         <v>66</v>
@@ -1698,7 +1698,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="8"/>
       <c r="B39" s="10" t="s">
         <v>68</v>
@@ -1711,9 +1711,9 @@
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>0</v>
@@ -1722,16 +1722,16 @@
         <v>1</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>2</v>
@@ -1740,7 +1740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" s="8"/>
       <c r="B41" s="2" t="s">
         <v>69</v>
@@ -1761,9 +1761,9 @@
       </c>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>73</v>
@@ -1784,7 +1784,7 @@
       </c>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" s="8"/>
       <c r="B43" s="2" t="s">
         <v>82</v>
@@ -1793,7 +1793,7 @@
         <v>84</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>11</v>
@@ -1807,7 +1807,7 @@
       </c>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="8"/>
       <c r="B44" s="2" t="s">
         <v>83</v>
@@ -1828,7 +1828,7 @@
       </c>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="8"/>
       <c r="B45" s="2" t="s">
         <v>77</v>
@@ -1851,7 +1851,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="8"/>
       <c r="B48" s="10" t="s">
         <v>80</v>
@@ -1864,9 +1864,9 @@
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>0</v>
@@ -1879,10 +1879,10 @@
         <v>7</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>2</v>
@@ -1891,9 +1891,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>86</v>
@@ -1907,14 +1907,14 @@
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I50" s="2"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="8"/>
       <c r="B51" s="2" t="s">
         <v>87</v>
@@ -1935,7 +1935,7 @@
       </c>
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="8"/>
       <c r="B52" s="2" t="s">
         <v>90</v>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="I52" s="2"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" s="8"/>
       <c r="B53" s="2" t="s">
         <v>94</v>
@@ -1979,7 +1979,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="8"/>
       <c r="B56" s="10" t="s">
         <v>97</v>
@@ -1992,9 +1992,9 @@
       <c r="H56" s="10"/>
       <c r="I56" s="10"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>0</v>
@@ -2003,16 +2003,16 @@
         <v>1</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>2</v>
@@ -2021,9 +2021,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>98</v>
@@ -2032,24 +2032,24 @@
         <v>99</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="H58" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="H58" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="I58" s="2"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" s="8"/>
       <c r="B59" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>99</v>
@@ -2063,14 +2063,14 @@
         <v>100</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I59" s="2"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" s="8"/>
       <c r="B60" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>99</v>
@@ -2080,21 +2080,21 @@
         <v>11</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G60" s="2"/>
       <c r="H60" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I60" s="2"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" s="8"/>
       <c r="B61" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2" t="s">
@@ -2105,14 +2105,14 @@
       </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I61" s="2"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" s="8"/>
       <c r="B62" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>99</v>
@@ -2122,20 +2122,20 @@
         <v>24</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G62" s="2"/>
       <c r="H62" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I62" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" s="8"/>
       <c r="B65" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C65" s="10"/>
       <c r="D65" s="10"/>
@@ -2145,9 +2145,9 @@
       <c r="H65" s="10"/>
       <c r="I65" s="10"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>0</v>
@@ -2160,10 +2160,10 @@
         <v>7</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>2</v>
@@ -2172,13 +2172,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" s="8"/>
       <c r="B67" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="2" t="s">
@@ -2186,20 +2186,20 @@
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I67" s="2"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" s="8"/>
       <c r="B68" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2" t="s">
@@ -2207,20 +2207,20 @@
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I68" s="2"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" s="8"/>
       <c r="B69" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2" t="s">
@@ -2231,58 +2231,58 @@
       </c>
       <c r="G69" s="2"/>
       <c r="H69" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I69" s="2"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" s="8"/>
       <c r="B70" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C70" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G70" s="2"/>
       <c r="H70" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I70" s="2"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" s="8"/>
       <c r="B71" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G71" s="2"/>
       <c r="H71" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I71" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" s="8"/>
       <c r="B74" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C74" s="10"/>
       <c r="D74" s="10"/>
@@ -2292,9 +2292,9 @@
       <c r="H74" s="10"/>
       <c r="I74" s="10"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>0</v>
@@ -2307,10 +2307,10 @@
         <v>7</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>2</v>
@@ -2319,13 +2319,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" s="8"/>
       <c r="B76" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C76" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="2" t="s">
@@ -2333,20 +2333,20 @@
       </c>
       <c r="F76" s="2"/>
       <c r="G76" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I76" s="2"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" s="8"/>
       <c r="B77" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="2" t="s">
@@ -2354,20 +2354,20 @@
       </c>
       <c r="F77" s="2"/>
       <c r="G77" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I77" s="2"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" s="8"/>
       <c r="B78" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2" t="s">
@@ -2378,58 +2378,58 @@
       </c>
       <c r="G78" s="2"/>
       <c r="H78" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I78" s="2"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" s="8"/>
       <c r="B79" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G79" s="2"/>
       <c r="H79" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I79" s="2"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" s="8"/>
       <c r="B80" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G80" s="2"/>
       <c r="H80" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I80" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A83" s="8"/>
       <c r="B83" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C83" s="10"/>
       <c r="D83" s="10"/>
@@ -2439,9 +2439,9 @@
       <c r="H83" s="10"/>
       <c r="I83" s="10"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A84" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>0</v>
@@ -2454,10 +2454,10 @@
         <v>7</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>2</v>
@@ -2466,15 +2466,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A85" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="2" t="s">
@@ -2482,68 +2482,68 @@
       </c>
       <c r="F85" s="2"/>
       <c r="G85" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I85" s="2"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A86" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C86" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="H85" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="I85" s="2"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G86" s="2"/>
       <c r="H86" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I86" s="2"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A87" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="I86" s="2"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>167</v>
       </c>
       <c r="D87" s="2"/>
       <c r="E87" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G87" s="2"/>
       <c r="H87" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I87" s="2"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A88" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" s="2" t="s">
@@ -2551,14 +2551,14 @@
       </c>
       <c r="F88" s="2"/>
       <c r="G88" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I88" s="2"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A89" s="8"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -2569,7 +2569,7 @@
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A90" s="8"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -2580,7 +2580,7 @@
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A91" s="8"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -2591,10 +2591,10 @@
       <c r="H91" s="2"/>
       <c r="I91" s="2"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A94" s="8"/>
       <c r="B94" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C94" s="10"/>
       <c r="D94" s="10"/>
@@ -2604,9 +2604,9 @@
       <c r="H94" s="10"/>
       <c r="I94" s="10"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A95" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>0</v>
@@ -2615,16 +2615,16 @@
         <v>1</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>2</v>
@@ -2633,16 +2633,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A96" s="8"/>
       <c r="B96" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D96" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>8</v>
@@ -2652,11 +2652,11 @@
         <v>31</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I96" s="2"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A97" s="8"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -2667,7 +2667,7 @@
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A98" s="8"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -2678,7 +2678,7 @@
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A99" s="8"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -2689,7 +2689,7 @@
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A100" s="8"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -2702,17 +2702,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B94:I94"/>
+    <mergeCell ref="B83:I83"/>
+    <mergeCell ref="B56:I56"/>
+    <mergeCell ref="B65:I65"/>
+    <mergeCell ref="B74:I74"/>
     <mergeCell ref="B48:I48"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B21:I21"/>
     <mergeCell ref="B30:I30"/>
     <mergeCell ref="B39:I39"/>
-    <mergeCell ref="B94:I94"/>
-    <mergeCell ref="B83:I83"/>
-    <mergeCell ref="B56:I56"/>
-    <mergeCell ref="B65:I65"/>
-    <mergeCell ref="B74:I74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2727,20 +2727,20 @@
       <selection sqref="A1:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.86328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -2749,7 +2749,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2772,50 +2772,50 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="B4" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>11</v>
@@ -2825,45 +2825,45 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="B7" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Realized get all students API
</commit_message>
<xml_diff>
--- a/API List.xlsx
+++ b/API List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DJ\Desktop\flaskAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA23B5C-0AAA-4A14-AE6B-E2EFFF196B53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995FAD15-751F-4B71-94FD-42FBF63500B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="833" yWindow="-98" windowWidth="18465" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="189">
   <si>
     <t>API Name</t>
   </si>
@@ -1010,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G52" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1022,7 +1022,7 @@
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="8.1328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.73046875" customWidth="1"/>
-    <col min="7" max="7" width="94.86328125" customWidth="1"/>
+    <col min="7" max="7" width="50.59765625" customWidth="1"/>
     <col min="8" max="8" width="47.59765625" customWidth="1"/>
     <col min="9" max="9" width="10.86328125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1118,7 +1118,9 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" s="8"/>
+      <c r="A5" s="8" t="s">
+        <v>154</v>
+      </c>
       <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
@@ -2702,17 +2704,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B94:I94"/>
-    <mergeCell ref="B83:I83"/>
-    <mergeCell ref="B56:I56"/>
-    <mergeCell ref="B65:I65"/>
-    <mergeCell ref="B74:I74"/>
     <mergeCell ref="B48:I48"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B21:I21"/>
     <mergeCell ref="B30:I30"/>
     <mergeCell ref="B39:I39"/>
+    <mergeCell ref="B94:I94"/>
+    <mergeCell ref="B83:I83"/>
+    <mergeCell ref="B56:I56"/>
+    <mergeCell ref="B65:I65"/>
+    <mergeCell ref="B74:I74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added attendance record to class sessions
</commit_message>
<xml_diff>
--- a/API List.xlsx
+++ b/API List.xlsx
@@ -805,10 +805,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J106"/>
+  <dimension ref="A1:J107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1094,142 +1094,134 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4"/>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4"/>
+      <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J17" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B18" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="5"/>
+      <c r="D18" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="E18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="G18" s="5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
+      <c r="J18" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4"/>
       <c r="B19" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="H19" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -1237,21 +1229,19 @@
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4"/>
       <c r="B20" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F20" s="5"/>
-      <c r="G20" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="G20" s="5"/>
       <c r="H20" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -1259,155 +1249,155 @@
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4"/>
       <c r="B21" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="D21" s="5"/>
       <c r="E21" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I21" s="5"/>
-      <c r="J21" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="J21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="A22" s="4"/>
       <c r="B22" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>29</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>59</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F22" s="5"/>
       <c r="G22" s="5" t="s">
         <v>47</v>
       </c>
       <c r="H22" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="E23" s="9"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="E24" s="9"/>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4"/>
-      <c r="B26" s="2" t="s">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="E25" s="9"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4"/>
+      <c r="B27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H28" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3" t="s">
+      <c r="I28" s="3"/>
+      <c r="J28" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B29" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="5"/>
+      <c r="D29" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="E29" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G29" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="H29" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
@@ -1415,19 +1405,21 @@
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4"/>
       <c r="B30" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F30" s="5"/>
+      <c r="F30" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="G30" s="5"/>
       <c r="H30" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
@@ -1435,23 +1427,19 @@
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4"/>
       <c r="B31" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>65</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
       <c r="H31" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
@@ -1459,161 +1447,163 @@
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4"/>
       <c r="B32" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>63</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G32" s="5"/>
+      <c r="G32" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="H32" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4"/>
+      <c r="B33" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5" t="s">
+      <c r="I33" s="5"/>
+      <c r="J33" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4"/>
-      <c r="B35" s="2" t="s">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4"/>
+      <c r="B36" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F37" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="G37" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="H37" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="3" t="s">
+      <c r="I37" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J36" s="3" t="s">
+      <c r="J37" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="s">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="4"/>
-      <c r="B38" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>79</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
+      <c r="G38" s="5" t="s">
+        <v>80</v>
+      </c>
       <c r="H38" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="A39" s="4"/>
       <c r="B39" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>86</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="D39" s="5"/>
       <c r="E39" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F39" s="5" t="s">
-        <v>38</v>
-      </c>
+      <c r="F39" s="5"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4"/>
+      <c r="A40" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="B40" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D40" s="5"/>
+        <v>85</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="E40" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5" t="s">
-        <v>65</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G40" s="5"/>
       <c r="H40" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
@@ -1621,62 +1611,56 @@
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4"/>
       <c r="B41" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>79</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4"/>
+      <c r="B42" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5" t="s">
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5" t="s">
+      <c r="I42" s="5"/>
+      <c r="J42" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>86</v>
@@ -1688,10 +1672,10 @@
         <v>38</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
@@ -1701,143 +1685,145 @@
         <v>10</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D44" s="5"/>
+        <v>97</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="E44" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G44" s="5"/>
+      <c r="G44" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="H44" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="I44" s="5" t="s">
+      <c r="I45" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="J44" s="5"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="4"/>
-      <c r="B47" s="2" t="s">
+      <c r="J45" s="5"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4"/>
+      <c r="B48" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="2" t="s">
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B49" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C49" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D49" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E49" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="F49" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G48" s="3" t="s">
+      <c r="G49" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H48" s="3" t="s">
+      <c r="H49" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3" t="s">
+      <c r="I49" s="3"/>
+      <c r="J49" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="4"/>
-      <c r="B49" s="5" t="s">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="4"/>
+      <c r="B50" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>109</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D50" s="5" t="s">
-        <v>110</v>
-      </c>
+      <c r="D50" s="5"/>
       <c r="E50" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>38</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F50" s="5"/>
       <c r="G50" s="5" t="s">
         <v>107</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="4"/>
+      <c r="A51" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="B51" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>38</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>19</v>
+        <v>107</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
@@ -1845,19 +1831,25 @@
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4"/>
       <c r="B52" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D52" s="5"/>
+        <v>113</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>114</v>
+      </c>
       <c r="E52" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
+      <c r="F52" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H52" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
@@ -1865,109 +1857,107 @@
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4"/>
       <c r="B53" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="D53" s="5"/>
       <c r="E53" s="5" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
       <c r="H53" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="4"/>
+      <c r="B54" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5" t="s">
+      <c r="I54" s="5"/>
+      <c r="J54" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="4"/>
-      <c r="B56" s="2" t="s">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="4"/>
+      <c r="B57" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="2" t="s">
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B58" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C58" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3" t="s">
+      <c r="D58" s="3"/>
+      <c r="E58" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="F58" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G57" s="3" t="s">
+      <c r="G58" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H57" s="3" t="s">
+      <c r="H58" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I57" s="3"/>
-      <c r="J57" s="3" t="s">
+      <c r="I58" s="3"/>
+      <c r="J58" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="4" t="s">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B59" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C59" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="H58" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="I58" s="5"/>
-      <c r="J58" s="5"/>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="4"/>
-      <c r="B59" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>127</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G59" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5" t="s">
+        <v>124</v>
+      </c>
       <c r="H59" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I59" s="5"/>
       <c r="J59" s="5"/>
@@ -1975,21 +1965,21 @@
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4"/>
       <c r="B60" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>131</v>
+        <v>19</v>
       </c>
       <c r="G60" s="5"/>
       <c r="H60" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="I60" s="5"/>
       <c r="J60" s="5"/>
@@ -1997,115 +1987,115 @@
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4"/>
       <c r="B61" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="5" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G61" s="5"/>
       <c r="H61" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="4"/>
+      <c r="B62" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="I61" s="5"/>
-      <c r="J61" s="5" t="s">
+      <c r="I62" s="5"/>
+      <c r="J62" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="4"/>
-      <c r="B64" s="2" t="s">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="4"/>
+      <c r="B65" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
-    </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="2" t="s">
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B66" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C66" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D66" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E65" s="3" t="s">
+      <c r="E66" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F65" s="3" t="s">
+      <c r="F66" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G65" s="3" t="s">
+      <c r="G66" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H65" s="3" t="s">
+      <c r="H66" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I65" s="3"/>
-      <c r="J65" s="3" t="s">
+      <c r="I66" s="3"/>
+      <c r="J66" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="4" t="s">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B67" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="H66" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="I66" s="5"/>
-      <c r="J66" s="5"/>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="4"/>
-      <c r="B67" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="D67" s="5"/>
+      <c r="D67" s="5" t="s">
+        <v>114</v>
+      </c>
       <c r="E67" s="5" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F67" s="5"/>
       <c r="G67" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
@@ -2113,21 +2103,21 @@
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="4"/>
       <c r="B68" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>138</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="G68" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5" t="s">
+        <v>142</v>
+      </c>
       <c r="H68" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I68" s="5"/>
       <c r="J68" s="5"/>
@@ -2135,21 +2125,21 @@
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="4"/>
       <c r="B69" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>68</v>
+        <v>145</v>
       </c>
       <c r="G69" s="5"/>
       <c r="H69" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I69" s="5"/>
       <c r="J69" s="5"/>
@@ -2157,109 +2147,109 @@
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="4"/>
       <c r="B70" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="5" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>145</v>
+        <v>68</v>
       </c>
       <c r="G70" s="5"/>
       <c r="H70" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="4"/>
+      <c r="B71" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="I70" s="5"/>
-      <c r="J70" s="5" t="s">
+      <c r="I71" s="5"/>
+      <c r="J71" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="4"/>
-      <c r="B73" s="2" t="s">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="4"/>
+      <c r="B74" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
-      <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
-      <c r="J73" s="2"/>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="2" t="s">
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B75" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="C75" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3" t="s">
+      <c r="D75" s="3"/>
+      <c r="E75" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F74" s="3" t="s">
+      <c r="F75" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G74" s="3" t="s">
+      <c r="G75" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H74" s="3" t="s">
+      <c r="H75" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I74" s="3"/>
-      <c r="J74" s="3" t="s">
+      <c r="I75" s="3"/>
+      <c r="J75" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="4"/>
-      <c r="B75" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="D75" s="5"/>
-      <c r="E75" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F75" s="5"/>
-      <c r="G75" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="H75" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="I75" s="5"/>
-      <c r="J75" s="5"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="4"/>
       <c r="B76" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>154</v>
       </c>
       <c r="D76" s="5"/>
       <c r="E76" s="5" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F76" s="5"/>
       <c r="G76" s="5" t="s">
         <v>155</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I76" s="5"/>
       <c r="J76" s="5"/>
@@ -2267,21 +2257,21 @@
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="4"/>
       <c r="B77" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G77" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5" t="s">
+        <v>155</v>
+      </c>
       <c r="H77" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I77" s="5"/>
       <c r="J77" s="5"/>
@@ -2289,21 +2279,21 @@
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="4"/>
       <c r="B78" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D78" s="5"/>
       <c r="E78" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>164</v>
+        <v>47</v>
       </c>
       <c r="G78" s="5"/>
       <c r="H78" s="5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="I78" s="5"/>
       <c r="J78" s="5"/>
@@ -2311,111 +2301,111 @@
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="4"/>
       <c r="B79" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="D79" s="5"/>
       <c r="E79" s="5" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G79" s="5"/>
       <c r="H79" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I79" s="5"/>
+      <c r="J79" s="5"/>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="4"/>
+      <c r="B80" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="G80" s="5"/>
+      <c r="H80" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="I79" s="5"/>
-      <c r="J79" s="5" t="s">
+      <c r="I80" s="5"/>
+      <c r="J80" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="4"/>
-      <c r="B82" s="2" t="s">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="4"/>
+      <c r="B83" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
-      <c r="E82" s="2"/>
-      <c r="F82" s="2"/>
-      <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
-      <c r="I82" s="2"/>
-      <c r="J82" s="2"/>
-    </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="2" t="s">
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2"/>
+      <c r="I83" s="2"/>
+      <c r="J83" s="2"/>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B84" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C84" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D83" s="3"/>
-      <c r="E83" s="3" t="s">
+      <c r="D84" s="3"/>
+      <c r="E84" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F83" s="3" t="s">
+      <c r="F84" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G83" s="3" t="s">
+      <c r="G84" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H83" s="3" t="s">
+      <c r="H84" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I83" s="3"/>
-      <c r="J83" s="3" t="s">
+      <c r="I84" s="3"/>
+      <c r="J84" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="4" t="s">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B85" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F84" s="5"/>
-      <c r="G84" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="H84" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="I84" s="5"/>
-      <c r="J84" s="5"/>
-    </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="4"/>
-      <c r="B85" s="5" t="s">
-        <v>174</v>
       </c>
       <c r="C85" s="5" t="s">
         <v>171</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="5" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F85" s="5"/>
       <c r="G85" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H85" s="5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="I85" s="5"/>
       <c r="J85" s="5"/>
@@ -2423,19 +2413,21 @@
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="4"/>
       <c r="B86" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="C86" s="5"/>
+        <v>174</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="D86" s="5"/>
       <c r="E86" s="5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F86" s="5"/>
       <c r="G86" s="5" t="s">
-        <v>19</v>
+        <v>175</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I86" s="5"/>
       <c r="J86" s="5"/>
@@ -2443,21 +2435,19 @@
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="4"/>
       <c r="B87" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>180</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="C87" s="5"/>
       <c r="D87" s="5"/>
       <c r="E87" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F87" s="5"/>
       <c r="G87" s="5" t="s">
-        <v>181</v>
+        <v>19</v>
       </c>
       <c r="H87" s="5" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I87" s="5"/>
       <c r="J87" s="5"/>
@@ -2465,115 +2455,113 @@
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="4"/>
       <c r="B88" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F88" s="5"/>
+      <c r="G88" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="H88" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="I88" s="5"/>
+      <c r="J88" s="5"/>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="4"/>
+      <c r="B89" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D89" s="5"/>
+      <c r="E89" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F88" s="5" t="s">
+      <c r="F89" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="G88" s="5"/>
-      <c r="H88" s="5" t="s">
+      <c r="G89" s="5"/>
+      <c r="H89" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="I88" s="5"/>
-      <c r="J88" s="5" t="s">
+      <c r="I89" s="5"/>
+      <c r="J89" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="4"/>
-      <c r="B91" s="2" t="s">
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="4"/>
+      <c r="B92" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
-      <c r="E91" s="2"/>
-      <c r="F91" s="2"/>
-      <c r="G91" s="2"/>
-      <c r="H91" s="2"/>
-      <c r="I91" s="2"/>
-      <c r="J91" s="2"/>
-    </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="2" t="s">
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="2"/>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B93" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C92" s="3" t="s">
+      <c r="C93" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D92" s="3"/>
-      <c r="E92" s="3" t="s">
+      <c r="D93" s="3"/>
+      <c r="E93" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F92" s="3" t="s">
+      <c r="F93" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G92" s="3" t="s">
+      <c r="G93" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H92" s="3" t="s">
+      <c r="H93" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I92" s="3" t="s">
+      <c r="I93" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J92" s="3" t="s">
+      <c r="J93" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D93" s="5"/>
-      <c r="E93" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F93" s="5"/>
-      <c r="G93" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="H93" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="I93" s="5"/>
-      <c r="J93" s="5"/>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D94" s="5"/>
       <c r="E94" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F94" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="G94" s="5"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5" t="s">
+        <v>188</v>
+      </c>
       <c r="H94" s="5" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="I94" s="5"/>
       <c r="J94" s="5"/>
@@ -2583,21 +2571,21 @@
         <v>10</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D95" s="5"/>
       <c r="E95" s="5" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>59</v>
+        <v>192</v>
       </c>
       <c r="G95" s="5"/>
       <c r="H95" s="5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="I95" s="5"/>
       <c r="J95" s="5"/>
@@ -2607,34 +2595,46 @@
         <v>10</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D96" s="5"/>
       <c r="E96" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F96" s="5"/>
-      <c r="G96" s="5" t="s">
-        <v>199</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G96" s="5"/>
       <c r="H96" s="5" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="I96" s="5"/>
       <c r="J96" s="5"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="4"/>
-      <c r="B97" s="5"/>
-      <c r="C97" s="5"/>
+      <c r="A97" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>198</v>
+      </c>
       <c r="D97" s="5"/>
-      <c r="E97" s="5"/>
+      <c r="E97" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="F97" s="5"/>
-      <c r="G97" s="5"/>
-      <c r="H97" s="5"/>
+      <c r="G97" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="H97" s="5" t="s">
+        <v>200</v>
+      </c>
       <c r="I97" s="5"/>
       <c r="J97" s="5"/>
     </row>
@@ -2662,83 +2662,83 @@
       <c r="I99" s="5"/>
       <c r="J99" s="5"/>
     </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="4"/>
-      <c r="B102" s="2" t="s">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="4"/>
+      <c r="B100" s="5"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="5"/>
+      <c r="G100" s="5"/>
+      <c r="H100" s="5"/>
+      <c r="I100" s="5"/>
+      <c r="J100" s="5"/>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="4"/>
+      <c r="B103" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C102" s="2"/>
-      <c r="D102" s="2"/>
-      <c r="E102" s="2"/>
-      <c r="F102" s="2"/>
-      <c r="G102" s="2"/>
-      <c r="H102" s="2"/>
-      <c r="I102" s="2"/>
-      <c r="J102" s="2"/>
-    </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="2" t="s">
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="2"/>
+      <c r="I103" s="2"/>
+      <c r="J103" s="2"/>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B103" s="3" t="s">
+      <c r="B104" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C103" s="3" t="s">
+      <c r="C104" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D103" s="3" t="s">
+      <c r="D104" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E103" s="3" t="s">
+      <c r="E104" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F103" s="3" t="s">
+      <c r="F104" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G103" s="3" t="s">
+      <c r="G104" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H103" s="3" t="s">
+      <c r="H104" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I103" s="3"/>
-      <c r="J103" s="3" t="s">
+      <c r="I104" s="3"/>
+      <c r="J104" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="4"/>
-      <c r="B104" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="C104" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="D104" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E104" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F104" s="5"/>
-      <c r="G104" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H104" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="I104" s="5"/>
-      <c r="J104" s="5"/>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="4"/>
-      <c r="B105" s="5"/>
-      <c r="C105" s="5"/>
-      <c r="D105" s="5"/>
-      <c r="E105" s="5"/>
+      <c r="B105" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="F105" s="5"/>
-      <c r="G105" s="5"/>
-      <c r="H105" s="5"/>
+      <c r="G105" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H105" s="5" t="s">
+        <v>204</v>
+      </c>
       <c r="I105" s="5"/>
       <c r="J105" s="5"/>
     </row>
@@ -2754,20 +2754,32 @@
       <c r="I106" s="5"/>
       <c r="J106" s="5"/>
     </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="4"/>
+      <c r="B107" s="5"/>
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="5"/>
+      <c r="F107" s="5"/>
+      <c r="G107" s="5"/>
+      <c r="H107" s="5"/>
+      <c r="I107" s="5"/>
+      <c r="J107" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="B10:J10"/>
-    <mergeCell ref="B15:J15"/>
-    <mergeCell ref="B26:J26"/>
-    <mergeCell ref="B35:J35"/>
-    <mergeCell ref="B47:J47"/>
-    <mergeCell ref="B56:J56"/>
-    <mergeCell ref="B64:J64"/>
-    <mergeCell ref="B73:J73"/>
-    <mergeCell ref="B82:J82"/>
-    <mergeCell ref="B91:J91"/>
-    <mergeCell ref="B102:J102"/>
+    <mergeCell ref="B16:J16"/>
+    <mergeCell ref="B27:J27"/>
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="B48:J48"/>
+    <mergeCell ref="B57:J57"/>
+    <mergeCell ref="B65:J65"/>
+    <mergeCell ref="B74:J74"/>
+    <mergeCell ref="B83:J83"/>
+    <mergeCell ref="B92:J92"/>
+    <mergeCell ref="B103:J103"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Implemented new class session recurring methods and updated DB design
</commit_message>
<xml_diff>
--- a/API List.xlsx
+++ b/API List.xlsx
@@ -440,7 +440,7 @@
     <t xml:space="preserve">/api/v1.0/class_session</t>
   </si>
   <si>
-    <t xml:space="preserve">course_id, start_time, duration, info, repeat_weekly, repeat_wkdays, repeat_until</t>
+    <t xml:space="preserve">course_id, start_time, end_time, duration, info, repeat_weekly, repeat_wkdays</t>
   </si>
   <si>
     <t xml:space="preserve">Add one class_session or repeating class_sessions</t>
@@ -807,8 +807,8 @@
   </sheetPr>
   <dimension ref="A1:J107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G67" activeCellId="0" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Implemented get user, get courses
</commit_message>
<xml_diff>
--- a/API List.xlsx
+++ b/API List.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="214">
   <si>
     <t xml:space="preserve">Students</t>
   </si>
@@ -50,6 +50,9 @@
     <t xml:space="preserve">Function</t>
   </si>
   <si>
+    <t xml:space="preserve">Return (JSON)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Comments</t>
   </si>
   <si>
@@ -125,9 +128,6 @@
     <t xml:space="preserve">Parents</t>
   </si>
   <si>
-    <t xml:space="preserve">Return (JSON)</t>
-  </si>
-  <si>
     <t xml:space="preserve">add_parent</t>
   </si>
   <si>
@@ -242,6 +242,9 @@
     <t xml:space="preserve">Get a list of all courses</t>
   </si>
   <si>
+    <t xml:space="preserve">[{id, name}]</t>
+  </si>
+  <si>
     <t xml:space="preserve">update_course</t>
   </si>
   <si>
@@ -272,7 +275,10 @@
     <t xml:space="preserve">get_user</t>
   </si>
   <si>
-    <t xml:space="preserve">Get one user</t>
+    <t xml:space="preserve">Get the user info based on access token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{id, realName, phone, email, roles, avatar, gender, language, city, provice, validated}</t>
   </si>
   <si>
     <t xml:space="preserve">get_unvalidated_users</t>
@@ -449,10 +455,16 @@
     <t xml:space="preserve">update_class_session</t>
   </si>
   <si>
-    <t xml:space="preserve">Teacher and above</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update a class_session's information</t>
+    <t xml:space="preserve">Update one class_session's information by admin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">update_class_sessions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/v1.0/class_sessions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update a series of class sessions by admin</t>
   </si>
   <si>
     <t xml:space="preserve">get_class_session</t>
@@ -464,9 +476,6 @@
     <t xml:space="preserve">get_class_sessions</t>
   </si>
   <si>
-    <t xml:space="preserve">/api/v1.0/class_sessions</t>
-  </si>
-  <si>
     <t xml:space="preserve">start_time, end_time</t>
   </si>
   <si>
@@ -476,6 +485,27 @@
     <t xml:space="preserve">[class_session]</t>
   </si>
   <si>
+    <t xml:space="preserve">teacher_update_class_session</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/v1.0/teacher_class_session</t>
+  </si>
+  <si>
+    <t xml:space="preserve">session_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teacher update his/her own one class session</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teacher_update_class_sessions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/v1.0/teacher_class_sessions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teacher update his/her own series of class sessions</t>
+  </si>
+  <si>
     <t xml:space="preserve">delete_class_session</t>
   </si>
   <si>
@@ -516,9 +546,6 @@
   </si>
   <si>
     <t xml:space="preserve">/api/v1.0/class_session_teachings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">session_id</t>
   </si>
   <si>
     <t xml:space="preserve">Get a list of teaching records by session_id</t>
@@ -645,7 +672,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -676,6 +703,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -685,7 +718,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -742,6 +775,13 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -768,7 +808,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -837,6 +877,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -858,17 +906,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:K108"/>
+  <dimension ref="B1:K111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B71" activeCellId="0" sqref="B71"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.13"/>
@@ -930,33 +978,35 @@
       <c r="I3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="6"/>
+      <c r="J3" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="K3" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="10"/>
@@ -964,47 +1014,47 @@
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="8"/>
       <c r="C5" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="10"/>
@@ -1012,23 +1062,23 @@
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="8"/>
       <c r="C7" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="10"/>
@@ -1036,27 +1086,27 @@
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="11"/>
       <c r="C8" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1085,7 +1135,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -1123,15 +1173,15 @@
         <v>8</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>35</v>
@@ -1143,7 +1193,7 @@
         <v>37</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>38</v>
@@ -1234,15 +1284,15 @@
         <v>8</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>43</v>
@@ -1254,7 +1304,7 @@
         <v>37</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>38</v>
@@ -1280,7 +1330,7 @@
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G20" s="9"/>
       <c r="H20" s="9" t="s">
@@ -1302,7 +1352,7 @@
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
@@ -1322,7 +1372,7 @@
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G22" s="9"/>
       <c r="H22" s="9" t="s">
@@ -1343,10 +1393,10 @@
         <v>44</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G23" s="9"/>
       <c r="H23" s="9" t="s">
@@ -1357,12 +1407,12 @@
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>57</v>
@@ -1371,10 +1421,10 @@
         <v>58</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>59</v>
@@ -1437,14 +1487,16 @@
       <c r="I29" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J29" s="6"/>
+      <c r="J29" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="K29" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>62</v>
@@ -1456,7 +1508,7 @@
         <v>64</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G30" s="9"/>
       <c r="H30" s="9" t="s">
@@ -1478,7 +1530,7 @@
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G31" s="9" t="s">
         <v>68</v>
@@ -1491,36 +1543,42 @@
       <c r="K31" s="10"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="8"/>
+      <c r="B32" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="C32" s="9" t="s">
         <v>70</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E32" s="9"/>
+      <c r="E32" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="F32" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
       <c r="I32" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="J32" s="9"/>
+      <c r="J32" s="9" t="s">
+        <v>73</v>
+      </c>
       <c r="K32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="8"/>
       <c r="C33" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>63</v>
       </c>
       <c r="E33" s="9"/>
       <c r="F33" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G33" s="9" t="s">
         <v>68</v>
@@ -1529,7 +1587,7 @@
         <v>65</v>
       </c>
       <c r="I33" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J33" s="9"/>
       <c r="K33" s="10"/>
@@ -1537,30 +1595,30 @@
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="11"/>
       <c r="C34" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>63</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G34" s="12" t="s">
         <v>68</v>
       </c>
       <c r="H34" s="12"/>
       <c r="I34" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J34" s="12"/>
       <c r="K34" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="15" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>
@@ -1598,78 +1656,86 @@
         <v>8</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="K38" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E39" s="9"/>
       <c r="F39" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G39" s="9"/>
       <c r="H39" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J39" s="9"/>
       <c r="K39" s="10"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="8"/>
+      <c r="B40" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="C40" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E40" s="9"/>
+        <v>80</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="F40" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G40" s="9"/>
+        <v>19</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="H40" s="9"/>
       <c r="I40" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="J40" s="9"/>
+        <v>84</v>
+      </c>
+      <c r="J40" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="K40" s="10"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G41" s="9" t="s">
         <v>38</v>
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J41" s="9"/>
       <c r="K41" s="10"/>
@@ -1677,21 +1743,21 @@
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="8"/>
       <c r="C42" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E42" s="9"/>
       <c r="F42" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G42" s="9"/>
       <c r="H42" s="9" t="s">
         <v>65</v>
       </c>
       <c r="I42" s="9" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J42" s="9"/>
       <c r="K42" s="10"/>
@@ -1699,110 +1765,110 @@
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="8"/>
       <c r="C43" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E43" s="9"/>
       <c r="F43" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
       <c r="I43" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="J43" s="9"/>
       <c r="K43" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>38</v>
       </c>
       <c r="H44" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J44" s="9"/>
       <c r="K44" s="10"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>38</v>
       </c>
       <c r="H45" s="9" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="I45" s="9" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J45" s="9"/>
       <c r="K45" s="10"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E46" s="12"/>
       <c r="F46" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G46" s="12" t="s">
         <v>38</v>
       </c>
       <c r="H46" s="12"/>
       <c r="I46" s="12" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J46" s="12" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="K46" s="13"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="15" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C49" s="15"/>
       <c r="D49" s="15"/>
@@ -1839,57 +1905,59 @@
       <c r="I50" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J50" s="6"/>
+      <c r="J50" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="K50" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="8"/>
       <c r="C51" s="9" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E51" s="9"/>
       <c r="F51" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G51" s="9"/>
       <c r="H51" s="9" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I51" s="9" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="J51" s="9"/>
       <c r="K51" s="10"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G52" s="9" t="s">
         <v>38</v>
       </c>
       <c r="H52" s="9" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I52" s="9" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J52" s="9"/>
       <c r="K52" s="10"/>
@@ -1897,25 +1965,25 @@
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="8"/>
       <c r="C53" s="9" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G53" s="9" t="s">
         <v>38</v>
       </c>
       <c r="H53" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I53" s="9" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="J53" s="9"/>
       <c r="K53" s="10"/>
@@ -1923,19 +1991,19 @@
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="8"/>
       <c r="C54" s="9" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E54" s="9"/>
       <c r="F54" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G54" s="9"/>
       <c r="H54" s="9"/>
       <c r="I54" s="9" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="J54" s="9"/>
       <c r="K54" s="10"/>
@@ -1943,38 +2011,38 @@
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="11"/>
       <c r="C55" s="12" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E55" s="12"/>
       <c r="F55" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G55" s="12"/>
       <c r="H55" s="12"/>
       <c r="I55" s="12" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J55" s="12"/>
       <c r="K55" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15"/>
-      <c r="F58" s="15"/>
-      <c r="G58" s="15"/>
-      <c r="H58" s="15"/>
-      <c r="I58" s="15"/>
-      <c r="J58" s="15"/>
-      <c r="K58" s="15"/>
+      <c r="B58" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
+      <c r="J58" s="17"/>
+      <c r="K58" s="17"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="5" t="s">
@@ -1986,7 +2054,9 @@
       <c r="D59" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E59" s="6"/>
+      <c r="E59" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="F59" s="6" t="s">
         <v>5</v>
       </c>
@@ -1999,31 +2069,33 @@
       <c r="I59" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J59" s="6"/>
+      <c r="J59" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="K59" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E60" s="9"/>
       <c r="F60" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G60" s="9"/>
       <c r="H60" s="9" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I60" s="9" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="J60" s="9"/>
       <c r="K60" s="10"/>
@@ -2031,21 +2103,21 @@
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="8"/>
       <c r="C61" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E61" s="9"/>
       <c r="F61" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H61" s="9"/>
       <c r="I61" s="9" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="J61" s="9"/>
       <c r="K61" s="10"/>
@@ -2053,21 +2125,21 @@
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="8"/>
       <c r="C62" s="9" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E62" s="9"/>
       <c r="F62" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H62" s="9"/>
       <c r="I62" s="9" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="J62" s="9"/>
       <c r="K62" s="10"/>
@@ -2075,30 +2147,30 @@
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="11"/>
       <c r="C63" s="12" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E63" s="12"/>
       <c r="F63" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G63" s="12" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H63" s="12"/>
       <c r="I63" s="12" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="J63" s="12"/>
       <c r="K63" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="15" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C66" s="15"/>
       <c r="D66" s="15"/>
@@ -2136,34 +2208,34 @@
         <v>8</v>
       </c>
       <c r="J67" s="6" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="K67" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G68" s="9"/>
       <c r="H68" s="9" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="I68" s="9" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="J68" s="9"/>
       <c r="K68" s="10"/>
@@ -2171,23 +2243,23 @@
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="8"/>
       <c r="C69" s="9" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>142</v>
+        <v>88</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G69" s="9" t="s">
         <v>38</v>
       </c>
       <c r="H69" s="9"/>
       <c r="I69" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J69" s="9"/>
       <c r="K69" s="10"/>
@@ -2195,345 +2267,359 @@
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="8"/>
       <c r="C70" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G70" s="9"/>
+        <v>26</v>
+      </c>
+      <c r="G70" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="H70" s="9"/>
       <c r="I70" s="9" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="J70" s="9"/>
       <c r="K70" s="10"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="B71" s="8"/>
       <c r="C71" s="9" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G71" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H71" s="9" t="s">
-        <v>148</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G71" s="9"/>
+      <c r="H71" s="9"/>
       <c r="I71" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="J71" s="9" t="s">
+      <c r="J71" s="9"/>
+      <c r="K71" s="10"/>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C72" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="K71" s="10"/>
-    </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="11"/>
-      <c r="C72" s="12" t="s">
+      <c r="D72" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H72" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="D72" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="E72" s="12"/>
-      <c r="F72" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="G72" s="12"/>
-      <c r="H72" s="12"/>
-      <c r="I72" s="12" t="s">
+      <c r="I72" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="J72" s="12"/>
-      <c r="K72" s="13" t="s">
-        <v>32</v>
-      </c>
+      <c r="J72" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="K72" s="10"/>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="8"/>
+      <c r="C73" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G73" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="I73" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="J73" s="9"/>
+      <c r="K73" s="10"/>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="8"/>
+      <c r="C74" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F74" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G74" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H74" s="9"/>
+      <c r="I74" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="J74" s="9"/>
+      <c r="K74" s="10"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="C75" s="15"/>
-      <c r="D75" s="15"/>
-      <c r="E75" s="15"/>
-      <c r="F75" s="15"/>
-      <c r="G75" s="15"/>
-      <c r="H75" s="15"/>
-      <c r="I75" s="15"/>
-      <c r="J75" s="15"/>
-      <c r="K75" s="15"/>
-    </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="5" t="s">
+      <c r="B75" s="11"/>
+      <c r="C75" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="D75" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G75" s="12"/>
+      <c r="H75" s="12"/>
+      <c r="I75" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="J75" s="12"/>
+      <c r="K75" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C78" s="15"/>
+      <c r="D78" s="15"/>
+      <c r="E78" s="15"/>
+      <c r="F78" s="15"/>
+      <c r="G78" s="15"/>
+      <c r="H78" s="15"/>
+      <c r="I78" s="15"/>
+      <c r="J78" s="15"/>
+      <c r="K78" s="15"/>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C76" s="6" t="s">
+      <c r="C79" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D76" s="6" t="s">
+      <c r="D79" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E76" s="6" t="s">
+      <c r="E79" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F76" s="6" t="s">
+      <c r="F79" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G76" s="6" t="s">
+      <c r="G79" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H76" s="6" t="s">
+      <c r="H79" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I76" s="6" t="s">
+      <c r="I79" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J76" s="6"/>
-      <c r="K76" s="7" t="s">
+      <c r="J79" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="8"/>
-      <c r="C77" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="D77" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="E77" s="9"/>
-      <c r="F77" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G77" s="9"/>
-      <c r="H77" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="I77" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="J77" s="9"/>
-      <c r="K77" s="10"/>
-    </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="8"/>
-      <c r="C78" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="D78" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="E78" s="9"/>
-      <c r="F78" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G78" s="9"/>
-      <c r="H78" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="I78" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="J78" s="9"/>
-      <c r="K78" s="10"/>
-    </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="8"/>
-      <c r="C79" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="D79" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="E79" s="9"/>
-      <c r="F79" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G79" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H79" s="9"/>
-      <c r="I79" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="J79" s="9"/>
-      <c r="K79" s="10"/>
+      <c r="K79" s="7" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="8"/>
       <c r="C80" s="9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E80" s="9"/>
       <c r="F80" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G80" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="H80" s="9"/>
+        <v>15</v>
+      </c>
+      <c r="G80" s="9"/>
+      <c r="H80" s="9" t="s">
+        <v>166</v>
+      </c>
       <c r="I80" s="9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J80" s="9"/>
       <c r="K80" s="10"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="11"/>
-      <c r="C81" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="D81" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="E81" s="12"/>
-      <c r="F81" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="G81" s="12" t="s">
+      <c r="B81" s="8"/>
+      <c r="C81" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="H81" s="12"/>
-      <c r="I81" s="12" t="s">
+      <c r="D81" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G81" s="9"/>
+      <c r="H81" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="I81" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="J81" s="12"/>
-      <c r="K81" s="13" t="s">
-        <v>32</v>
-      </c>
+      <c r="J81" s="9"/>
+      <c r="K81" s="10"/>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="8"/>
+      <c r="C82" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D82" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G82" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H82" s="9"/>
+      <c r="I82" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="J82" s="9"/>
+      <c r="K82" s="10"/>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="8"/>
+      <c r="C83" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D83" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G83" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="H83" s="9"/>
+      <c r="I83" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="J83" s="9"/>
+      <c r="K83" s="10"/>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="C84" s="15"/>
-      <c r="D84" s="15"/>
-      <c r="E84" s="15"/>
-      <c r="F84" s="15"/>
-      <c r="G84" s="15"/>
-      <c r="H84" s="15"/>
-      <c r="I84" s="15"/>
-      <c r="J84" s="15"/>
-      <c r="K84" s="15"/>
-    </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="5" t="s">
+      <c r="B84" s="11"/>
+      <c r="C84" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="D84" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G84" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="H84" s="12"/>
+      <c r="I84" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="J84" s="12"/>
+      <c r="K84" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B87" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="C87" s="15"/>
+      <c r="D87" s="15"/>
+      <c r="E87" s="15"/>
+      <c r="F87" s="15"/>
+      <c r="G87" s="15"/>
+      <c r="H87" s="15"/>
+      <c r="I87" s="15"/>
+      <c r="J87" s="15"/>
+      <c r="K87" s="15"/>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B88" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C85" s="6" t="s">
+      <c r="C88" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D85" s="6" t="s">
+      <c r="D88" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E85" s="6" t="s">
+      <c r="E88" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F85" s="6" t="s">
+      <c r="F88" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G85" s="6" t="s">
+      <c r="G88" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H85" s="6" t="s">
+      <c r="H88" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I85" s="6" t="s">
+      <c r="I88" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J85" s="6"/>
-      <c r="K85" s="7" t="s">
+      <c r="J88" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="8" t="s">
+      <c r="K88" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C86" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="D86" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="E86" s="9"/>
-      <c r="F86" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G86" s="9"/>
-      <c r="H86" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="I86" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="J86" s="9"/>
-      <c r="K86" s="10"/>
-    </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="8"/>
-      <c r="C87" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="D87" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="E87" s="9"/>
-      <c r="F87" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G87" s="9"/>
-      <c r="H87" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="I87" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="J87" s="9"/>
-      <c r="K87" s="10"/>
-    </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="8"/>
-      <c r="C88" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="D88" s="9"/>
-      <c r="E88" s="9"/>
-      <c r="F88" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G88" s="9"/>
-      <c r="H88" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I88" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="J88" s="9"/>
-      <c r="K88" s="10"/>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="8"/>
+      <c r="B89" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="C89" s="9" t="s">
         <v>180</v>
       </c>
@@ -2542,7 +2628,7 @@
       </c>
       <c r="E89" s="9"/>
       <c r="F89" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G89" s="9"/>
       <c r="H89" s="9" t="s">
@@ -2555,294 +2641,362 @@
       <c r="K89" s="10"/>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="11"/>
-      <c r="C90" s="12" t="s">
+      <c r="B90" s="8"/>
+      <c r="C90" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="D90" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="E90" s="12"/>
-      <c r="F90" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="G90" s="12"/>
-      <c r="H90" s="12"/>
-      <c r="I90" s="12" t="s">
+      <c r="D90" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E90" s="9"/>
+      <c r="F90" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G90" s="9"/>
+      <c r="H90" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="J90" s="12"/>
-      <c r="K90" s="13" t="s">
-        <v>32</v>
-      </c>
+      <c r="I90" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="J90" s="9"/>
+      <c r="K90" s="10"/>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="8"/>
+      <c r="C91" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G91" s="9"/>
+      <c r="H91" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I91" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="J91" s="9"/>
+      <c r="K91" s="10"/>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B92" s="8"/>
+      <c r="C92" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D92" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G92" s="9"/>
+      <c r="H92" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="I92" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="J92" s="9"/>
+      <c r="K92" s="10"/>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="15" t="s">
+      <c r="B93" s="11"/>
+      <c r="C93" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="D93" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="E93" s="12"/>
+      <c r="F93" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G93" s="12"/>
+      <c r="H93" s="12"/>
+      <c r="I93" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="J93" s="12"/>
+      <c r="K93" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B96" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C93" s="15"/>
-      <c r="D93" s="15"/>
-      <c r="E93" s="15"/>
-      <c r="F93" s="15"/>
-      <c r="G93" s="15"/>
-      <c r="H93" s="15"/>
-      <c r="I93" s="15"/>
-      <c r="J93" s="15"/>
-      <c r="K93" s="15"/>
-    </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="5" t="s">
+      <c r="C96" s="15"/>
+      <c r="D96" s="15"/>
+      <c r="E96" s="15"/>
+      <c r="F96" s="15"/>
+      <c r="G96" s="15"/>
+      <c r="H96" s="15"/>
+      <c r="I96" s="15"/>
+      <c r="J96" s="15"/>
+      <c r="K96" s="15"/>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B97" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C94" s="6" t="s">
+      <c r="C97" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D94" s="6" t="s">
+      <c r="D97" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E94" s="6"/>
-      <c r="F94" s="6" t="s">
+      <c r="E97" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F97" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G94" s="6" t="s">
+      <c r="G97" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H94" s="6" t="s">
+      <c r="H97" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I94" s="6" t="s">
+      <c r="I97" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J94" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K94" s="7" t="s">
+      <c r="J97" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="8" t="s">
+      <c r="K97" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C95" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="D95" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="E95" s="9"/>
-      <c r="F95" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G95" s="9"/>
-      <c r="H95" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="I95" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="J95" s="9"/>
-      <c r="K95" s="10"/>
-    </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="8" t="s">
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B98" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C98" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="D98" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="E98" s="9"/>
+      <c r="F98" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G98" s="9"/>
+      <c r="H98" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="I98" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="J98" s="9"/>
+      <c r="K98" s="10"/>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B99" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C99" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="D99" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E99" s="9"/>
+      <c r="F99" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G99" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="H99" s="9"/>
+      <c r="I99" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="J99" s="9"/>
+      <c r="K99" s="10"/>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B100" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="D100" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="E100" s="9"/>
+      <c r="F100" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G100" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H100" s="9"/>
+      <c r="I100" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="J100" s="9"/>
+      <c r="K100" s="10"/>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B101" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C101" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="D101" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="E101" s="12"/>
+      <c r="F101" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G101" s="12"/>
+      <c r="H101" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="I101" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="J101" s="12"/>
+      <c r="K101" s="13"/>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B102" s="14"/>
+      <c r="C102" s="9"/>
+      <c r="D102" s="9"/>
+      <c r="E102" s="9"/>
+      <c r="F102" s="9"/>
+      <c r="G102" s="9"/>
+      <c r="H102" s="9"/>
+      <c r="I102" s="9"/>
+      <c r="J102" s="9"/>
+      <c r="K102" s="9"/>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B103" s="14"/>
+      <c r="C103" s="9"/>
+      <c r="D103" s="9"/>
+      <c r="E103" s="9"/>
+      <c r="F103" s="9"/>
+      <c r="G103" s="9"/>
+      <c r="H103" s="9"/>
+      <c r="I103" s="9"/>
+      <c r="J103" s="9"/>
+      <c r="K103" s="9"/>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B104" s="14"/>
+      <c r="C104" s="9"/>
+      <c r="D104" s="9"/>
+      <c r="E104" s="9"/>
+      <c r="F104" s="9"/>
+      <c r="G104" s="9"/>
+      <c r="H104" s="9"/>
+      <c r="I104" s="9"/>
+      <c r="J104" s="9"/>
+      <c r="K104" s="9"/>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B107" s="19"/>
+      <c r="C107" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D107" s="4"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="4"/>
+      <c r="G107" s="4"/>
+      <c r="H107" s="4"/>
+      <c r="I107" s="4"/>
+      <c r="J107" s="4"/>
+      <c r="K107" s="4"/>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B108" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D108" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E108" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F108" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G108" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H108" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I108" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J108" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K108" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C96" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="D96" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="E96" s="9"/>
-      <c r="F96" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G96" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="H96" s="9"/>
-      <c r="I96" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="J96" s="9"/>
-      <c r="K96" s="10"/>
-    </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C97" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="D97" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="E97" s="9"/>
-      <c r="F97" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G97" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="H97" s="9"/>
-      <c r="I97" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="J97" s="9"/>
-      <c r="K97" s="10"/>
-    </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C98" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="D98" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="E98" s="12"/>
-      <c r="F98" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G98" s="12"/>
-      <c r="H98" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="I98" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="J98" s="12"/>
-      <c r="K98" s="13"/>
-    </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="14"/>
-      <c r="C99" s="9"/>
-      <c r="D99" s="9"/>
-      <c r="E99" s="9"/>
-      <c r="F99" s="9"/>
-      <c r="G99" s="9"/>
-      <c r="H99" s="9"/>
-      <c r="I99" s="9"/>
-      <c r="J99" s="9"/>
-      <c r="K99" s="9"/>
-    </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="14"/>
-      <c r="C100" s="9"/>
-      <c r="D100" s="9"/>
-      <c r="E100" s="9"/>
-      <c r="F100" s="9"/>
-      <c r="G100" s="9"/>
-      <c r="H100" s="9"/>
-      <c r="I100" s="9"/>
-      <c r="J100" s="9"/>
-      <c r="K100" s="9"/>
-    </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="14"/>
-      <c r="C101" s="9"/>
-      <c r="D101" s="9"/>
-      <c r="E101" s="9"/>
-      <c r="F101" s="9"/>
-      <c r="G101" s="9"/>
-      <c r="H101" s="9"/>
-      <c r="I101" s="9"/>
-      <c r="J101" s="9"/>
-      <c r="K101" s="9"/>
-    </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="17"/>
-      <c r="C104" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="D104" s="4"/>
-      <c r="E104" s="4"/>
-      <c r="F104" s="4"/>
-      <c r="G104" s="4"/>
-      <c r="H104" s="4"/>
-      <c r="I104" s="4"/>
-      <c r="J104" s="4"/>
-      <c r="K104" s="4"/>
-    </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C105" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D105" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E105" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F105" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G105" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H105" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I105" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J105" s="6"/>
-      <c r="K105" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B106" s="11"/>
-      <c r="C106" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="D106" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="E106" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="F106" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G106" s="12"/>
-      <c r="H106" s="12" t="s">
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B109" s="11"/>
+      <c r="C109" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="D109" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="E109" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F109" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G109" s="12"/>
+      <c r="H109" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="I106" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="J106" s="12"/>
-      <c r="K106" s="13"/>
-    </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="14"/>
-      <c r="C107" s="9"/>
-      <c r="D107" s="9"/>
-      <c r="E107" s="9"/>
-      <c r="F107" s="9"/>
-      <c r="G107" s="9"/>
-      <c r="H107" s="9"/>
-      <c r="I107" s="9"/>
-      <c r="J107" s="9"/>
-      <c r="K107" s="9"/>
-    </row>
-    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="14"/>
-      <c r="C108" s="9"/>
-      <c r="D108" s="9"/>
-      <c r="E108" s="9"/>
-      <c r="F108" s="9"/>
-      <c r="G108" s="9"/>
-      <c r="H108" s="9"/>
-      <c r="I108" s="9"/>
-      <c r="J108" s="9"/>
-      <c r="K108" s="9"/>
+      <c r="I109" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="J109" s="12"/>
+      <c r="K109" s="13"/>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B110" s="14"/>
+      <c r="C110" s="9"/>
+      <c r="D110" s="9"/>
+      <c r="E110" s="9"/>
+      <c r="F110" s="9"/>
+      <c r="G110" s="9"/>
+      <c r="H110" s="9"/>
+      <c r="I110" s="9"/>
+      <c r="J110" s="9"/>
+      <c r="K110" s="9"/>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B111" s="14"/>
+      <c r="C111" s="9"/>
+      <c r="D111" s="9"/>
+      <c r="E111" s="9"/>
+      <c r="F111" s="9"/>
+      <c r="G111" s="9"/>
+      <c r="H111" s="9"/>
+      <c r="I111" s="9"/>
+      <c r="J111" s="9"/>
+      <c r="K111" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2854,10 +3008,10 @@
     <mergeCell ref="B49:K49"/>
     <mergeCell ref="B58:K58"/>
     <mergeCell ref="B66:K66"/>
-    <mergeCell ref="B75:K75"/>
-    <mergeCell ref="B84:K84"/>
-    <mergeCell ref="B93:K93"/>
-    <mergeCell ref="C104:K104"/>
+    <mergeCell ref="B78:K78"/>
+    <mergeCell ref="B87:K87"/>
+    <mergeCell ref="B96:K96"/>
+    <mergeCell ref="C107:K107"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
changed get class session to POST
</commit_message>
<xml_diff>
--- a/API List.xlsx
+++ b/API List.xlsx
@@ -672,7 +672,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -702,12 +702,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -808,7 +802,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -881,10 +875,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -908,8 +898,8 @@
   </sheetPr>
   <dimension ref="B1:K111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F72" activeCellId="0" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2324,7 +2314,7 @@
         <v>116</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G72" s="9" t="s">
         <v>38</v>
@@ -2384,7 +2374,7 @@
         <v>38</v>
       </c>
       <c r="H74" s="9"/>
-      <c r="I74" s="18" t="s">
+      <c r="I74" s="9" t="s">
         <v>160</v>
       </c>
       <c r="J74" s="9"/>
@@ -2905,7 +2895,7 @@
       <c r="K104" s="9"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="19"/>
+      <c r="B107" s="18"/>
       <c r="C107" s="4" t="s">
         <v>210</v>
       </c>

</xml_diff>

<commit_message>
Realized get parents of a student API
</commit_message>
<xml_diff>
--- a/API List.xlsx
+++ b/API List.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="218">
   <si>
     <t xml:space="preserve">Students</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t xml:space="preserve">Get a list of parents of the student</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{parent_name, relation}]</t>
   </si>
   <si>
     <t xml:space="preserve">Parents</t>
@@ -927,7 +930,7 @@
   <dimension ref="B1:K115"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1128,7 +1131,9 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="C9" s="6" t="s">
         <v>34</v>
       </c>
@@ -1148,7 +1153,9 @@
       <c r="I9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="6"/>
+      <c r="J9" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="K9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1189,7 +1196,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -1238,29 +1245,29 @@
         <v>11</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F15" s="14" t="s">
         <v>15</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J15" s="14"/>
       <c r="K15" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1269,7 +1276,7 @@
         <v>22</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E16" s="14" t="s">
         <v>36</v>
@@ -1278,11 +1285,11 @@
         <v>19</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J16" s="14"/>
       <c r="K16" s="15"/>
@@ -1336,7 +1343,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -1385,38 +1392,38 @@
         <v>11</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="17"/>
       <c r="C24" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8" t="s">
@@ -1424,10 +1431,10 @@
       </c>
       <c r="G24" s="8"/>
       <c r="H24" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J24" s="8"/>
       <c r="K24" s="18"/>
@@ -1435,10 +1442,10 @@
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="17"/>
       <c r="C25" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8" t="s">
@@ -1447,7 +1454,7 @@
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J25" s="8"/>
       <c r="K25" s="18"/>
@@ -1455,10 +1462,10 @@
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="17"/>
       <c r="C26" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8" t="s">
@@ -1466,10 +1473,10 @@
       </c>
       <c r="G26" s="8"/>
       <c r="H26" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J26" s="8"/>
       <c r="K26" s="18"/>
@@ -1477,10 +1484,10 @@
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="17"/>
       <c r="C27" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>30</v>
@@ -1490,10 +1497,10 @@
       </c>
       <c r="G27" s="8"/>
       <c r="H27" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J27" s="8"/>
       <c r="K27" s="18" t="s">
@@ -1505,10 +1512,10 @@
         <v>11</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E28" s="14" t="s">
         <v>30</v>
@@ -1517,13 +1524,13 @@
         <v>15</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I28" s="14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J28" s="14"/>
       <c r="K28" s="15"/>
@@ -1540,7 +1547,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -1589,23 +1596,23 @@
         <v>11</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J34" s="8"/>
       <c r="K34" s="18"/>
@@ -1613,21 +1620,21 @@
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="17"/>
       <c r="C35" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8" t="s">
         <v>19</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H35" s="8"/>
       <c r="I35" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J35" s="8"/>
       <c r="K35" s="18"/>
@@ -1637,13 +1644,13 @@
         <v>11</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>19</v>
@@ -1651,33 +1658,33 @@
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
       <c r="I36" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K36" s="18"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="17"/>
       <c r="C37" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J37" s="8"/>
       <c r="K37" s="18"/>
@@ -1685,21 +1692,21 @@
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="13"/>
       <c r="C38" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E38" s="14"/>
       <c r="F38" s="14" t="s">
         <v>31</v>
       </c>
       <c r="G38" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H38" s="14"/>
       <c r="I38" s="14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J38" s="14"/>
       <c r="K38" s="15" t="s">
@@ -1708,7 +1715,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
@@ -1757,10 +1764,10 @@
         <v>11</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="8" t="s">
@@ -1768,10 +1775,10 @@
       </c>
       <c r="G43" s="8"/>
       <c r="H43" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J43" s="8"/>
       <c r="K43" s="18"/>
@@ -1781,26 +1788,26 @@
         <v>11</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F44" s="8" t="s">
         <v>19</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H44" s="8"/>
       <c r="I44" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J44" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K44" s="18"/>
     </row>
@@ -1809,23 +1816,23 @@
         <v>11</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>19</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H45" s="8"/>
       <c r="I45" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="18"/>
@@ -1833,10 +1840,10 @@
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="17"/>
       <c r="C46" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E46" s="8"/>
       <c r="F46" s="8" t="s">
@@ -1844,10 +1851,10 @@
       </c>
       <c r="G46" s="8"/>
       <c r="H46" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J46" s="8"/>
       <c r="K46" s="18"/>
@@ -1855,10 +1862,10 @@
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="17"/>
       <c r="C47" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E47" s="8"/>
       <c r="F47" s="8" t="s">
@@ -1867,7 +1874,7 @@
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
       <c r="I47" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J47" s="8"/>
       <c r="K47" s="18" t="s">
@@ -1879,25 +1886,25 @@
         <v>11</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F48" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J48" s="8"/>
       <c r="K48" s="18"/>
@@ -1907,25 +1914,25 @@
         <v>11</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H49" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J49" s="8"/>
       <c r="K49" s="18"/>
@@ -1935,30 +1942,30 @@
         <v>11</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E50" s="14"/>
       <c r="F50" s="14" t="s">
         <v>19</v>
       </c>
       <c r="G50" s="14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H50" s="14"/>
       <c r="I50" s="14" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J50" s="14" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="K50" s="15"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
@@ -2005,10 +2012,10 @@
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="17"/>
       <c r="C55" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E55" s="8"/>
       <c r="F55" s="8" t="s">
@@ -2016,10 +2023,10 @@
       </c>
       <c r="G55" s="8"/>
       <c r="H55" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J55" s="8"/>
       <c r="K55" s="18"/>
@@ -2029,25 +2036,25 @@
         <v>11</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F56" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H56" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J56" s="8"/>
       <c r="K56" s="18"/>
@@ -2055,10 +2062,10 @@
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="17"/>
       <c r="C57" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>14</v>
@@ -2067,13 +2074,13 @@
         <v>19</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H57" s="8" t="s">
         <v>20</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J57" s="8"/>
       <c r="K57" s="18"/>
@@ -2081,10 +2088,10 @@
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="17"/>
       <c r="C58" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E58" s="8"/>
       <c r="F58" s="8" t="s">
@@ -2093,7 +2100,7 @@
       <c r="G58" s="8"/>
       <c r="H58" s="8"/>
       <c r="I58" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J58" s="8"/>
       <c r="K58" s="18"/>
@@ -2101,10 +2108,10 @@
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="13"/>
       <c r="C59" s="14" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E59" s="14"/>
       <c r="F59" s="14" t="s">
@@ -2113,7 +2120,7 @@
       <c r="G59" s="14"/>
       <c r="H59" s="14"/>
       <c r="I59" s="14" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="J59" s="14"/>
       <c r="K59" s="15" t="s">
@@ -2122,7 +2129,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="19" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C62" s="19"/>
       <c r="D62" s="19"/>
@@ -2171,10 +2178,10 @@
         <v>11</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>36</v>
@@ -2183,13 +2190,13 @@
         <v>15</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H64" s="8" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I64" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J64" s="8"/>
       <c r="K64" s="18"/>
@@ -2197,10 +2204,10 @@
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="17"/>
       <c r="C65" s="8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E65" s="8"/>
       <c r="F65" s="8" t="s">
@@ -2209,7 +2216,7 @@
       <c r="G65" s="8"/>
       <c r="H65" s="8"/>
       <c r="I65" s="8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J65" s="8"/>
       <c r="K65" s="18"/>
@@ -2217,10 +2224,10 @@
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="17"/>
       <c r="C66" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E66" s="8"/>
       <c r="F66" s="8" t="s">
@@ -2229,7 +2236,7 @@
       <c r="G66" s="8"/>
       <c r="H66" s="8"/>
       <c r="I66" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J66" s="8"/>
       <c r="K66" s="18"/>
@@ -2237,10 +2244,10 @@
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="13"/>
       <c r="C67" s="14" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E67" s="14"/>
       <c r="F67" s="14" t="s">
@@ -2249,7 +2256,7 @@
       <c r="G67" s="14"/>
       <c r="H67" s="14"/>
       <c r="I67" s="14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J67" s="14"/>
       <c r="K67" s="15" t="s">
@@ -2258,7 +2265,7 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C70" s="9"/>
       <c r="D70" s="9"/>
@@ -2307,10 +2314,10 @@
         <v>11</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>14</v>
@@ -2320,10 +2327,10 @@
       </c>
       <c r="G72" s="8"/>
       <c r="H72" s="8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I72" s="8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="J72" s="8"/>
       <c r="K72" s="18"/>
@@ -2331,23 +2338,23 @@
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="17"/>
       <c r="C73" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F73" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H73" s="8"/>
       <c r="I73" s="8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J73" s="8"/>
       <c r="K73" s="18"/>
@@ -2355,23 +2362,23 @@
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="17"/>
       <c r="C74" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F74" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G74" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H74" s="8"/>
       <c r="I74" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J74" s="8"/>
       <c r="K74" s="18"/>
@@ -2379,10 +2386,10 @@
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="17"/>
       <c r="C75" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E75" s="8" t="s">
         <v>14</v>
@@ -2393,7 +2400,7 @@
       <c r="G75" s="8"/>
       <c r="H75" s="8"/>
       <c r="I75" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="J75" s="8"/>
       <c r="K75" s="18"/>
@@ -2403,10 +2410,10 @@
         <v>11</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>14</v>
@@ -2415,26 +2422,26 @@
         <v>15</v>
       </c>
       <c r="G76" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H76" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I76" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J76" s="8" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="K76" s="18"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="17"/>
       <c r="C77" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E77" s="8" t="s">
         <v>14</v>
@@ -2443,13 +2450,13 @@
         <v>26</v>
       </c>
       <c r="G77" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H77" s="8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I77" s="8" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="J77" s="8"/>
       <c r="K77" s="18"/>
@@ -2457,10 +2464,10 @@
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="17"/>
       <c r="C78" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E78" s="8" t="s">
         <v>14</v>
@@ -2469,11 +2476,11 @@
         <v>26</v>
       </c>
       <c r="G78" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H78" s="8"/>
       <c r="I78" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J78" s="8"/>
       <c r="K78" s="18"/>
@@ -2481,10 +2488,10 @@
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="13"/>
       <c r="C79" s="14" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E79" s="14"/>
       <c r="F79" s="14" t="s">
@@ -2493,7 +2500,7 @@
       <c r="G79" s="14"/>
       <c r="H79" s="14"/>
       <c r="I79" s="14" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J79" s="14"/>
       <c r="K79" s="15" t="s">
@@ -2502,7 +2509,7 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C82" s="9"/>
       <c r="D82" s="9"/>
@@ -2549,10 +2556,10 @@
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="17"/>
       <c r="C84" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E84" s="8"/>
       <c r="F84" s="8" t="s">
@@ -2560,10 +2567,10 @@
       </c>
       <c r="G84" s="8"/>
       <c r="H84" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I84" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="J84" s="8"/>
       <c r="K84" s="18"/>
@@ -2571,10 +2578,10 @@
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="17"/>
       <c r="C85" s="8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E85" s="8"/>
       <c r="F85" s="8" t="s">
@@ -2582,10 +2589,10 @@
       </c>
       <c r="G85" s="8"/>
       <c r="H85" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I85" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J85" s="8"/>
       <c r="K85" s="18"/>
@@ -2593,21 +2600,21 @@
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="17"/>
       <c r="C86" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E86" s="8"/>
       <c r="F86" s="8" t="s">
         <v>19</v>
       </c>
       <c r="G86" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H86" s="8"/>
       <c r="I86" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J86" s="8"/>
       <c r="K86" s="18"/>
@@ -2615,21 +2622,21 @@
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="17"/>
       <c r="C87" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E87" s="8"/>
       <c r="F87" s="8" t="s">
         <v>19</v>
       </c>
       <c r="G87" s="8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H87" s="8"/>
       <c r="I87" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J87" s="8"/>
       <c r="K87" s="18"/>
@@ -2637,21 +2644,21 @@
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="13"/>
       <c r="C88" s="14" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E88" s="14"/>
       <c r="F88" s="14" t="s">
         <v>31</v>
       </c>
       <c r="G88" s="14" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H88" s="14"/>
       <c r="I88" s="14" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="J88" s="14"/>
       <c r="K88" s="15" t="s">
@@ -2660,7 +2667,7 @@
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C91" s="9"/>
       <c r="D91" s="9"/>
@@ -2709,10 +2716,10 @@
         <v>11</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E93" s="8"/>
       <c r="F93" s="8" t="s">
@@ -2720,10 +2727,10 @@
       </c>
       <c r="G93" s="8"/>
       <c r="H93" s="8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I93" s="8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J93" s="8"/>
       <c r="K93" s="18"/>
@@ -2731,10 +2738,10 @@
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="17"/>
       <c r="C94" s="8" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E94" s="8"/>
       <c r="F94" s="8" t="s">
@@ -2742,10 +2749,10 @@
       </c>
       <c r="G94" s="8"/>
       <c r="H94" s="8" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I94" s="8" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="J94" s="8"/>
       <c r="K94" s="18"/>
@@ -2753,7 +2760,7 @@
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="17"/>
       <c r="C95" s="8" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D95" s="8"/>
       <c r="E95" s="8"/>
@@ -2765,7 +2772,7 @@
         <v>20</v>
       </c>
       <c r="I95" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J95" s="8"/>
       <c r="K95" s="18"/>
@@ -2773,10 +2780,10 @@
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="17"/>
       <c r="C96" s="8" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E96" s="8"/>
       <c r="F96" s="8" t="s">
@@ -2784,10 +2791,10 @@
       </c>
       <c r="G96" s="8"/>
       <c r="H96" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I96" s="8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="J96" s="8"/>
       <c r="K96" s="18"/>
@@ -2795,10 +2802,10 @@
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="13"/>
       <c r="C97" s="14" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D97" s="14" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E97" s="14"/>
       <c r="F97" s="14" t="s">
@@ -2807,7 +2814,7 @@
       <c r="G97" s="14"/>
       <c r="H97" s="14"/>
       <c r="I97" s="14" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J97" s="14"/>
       <c r="K97" s="15" t="s">
@@ -2816,7 +2823,7 @@
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C100" s="9"/>
       <c r="D100" s="9"/>
@@ -2865,10 +2872,10 @@
         <v>11</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D102" s="8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E102" s="8"/>
       <c r="F102" s="8" t="s">
@@ -2876,10 +2883,10 @@
       </c>
       <c r="G102" s="8"/>
       <c r="H102" s="8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I102" s="8" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J102" s="8"/>
       <c r="K102" s="18"/>
@@ -2889,21 +2896,21 @@
         <v>11</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E103" s="8"/>
       <c r="F103" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G103" s="8" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H103" s="8"/>
       <c r="I103" s="8" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="J103" s="8"/>
       <c r="K103" s="18"/>
@@ -2913,21 +2920,21 @@
         <v>11</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E104" s="8"/>
       <c r="F104" s="8" t="s">
         <v>31</v>
       </c>
       <c r="G104" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H104" s="8"/>
       <c r="I104" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="J104" s="8"/>
       <c r="K104" s="18"/>
@@ -2937,10 +2944,10 @@
         <v>11</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D105" s="14" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E105" s="14"/>
       <c r="F105" s="14" t="s">
@@ -2948,10 +2955,10 @@
       </c>
       <c r="G105" s="14"/>
       <c r="H105" s="14" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I105" s="14" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="J105" s="14"/>
       <c r="K105" s="15"/>
@@ -2995,7 +3002,7 @@
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="20"/>
       <c r="C111" s="21" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D111" s="21"/>
       <c r="E111" s="21"/>
@@ -3041,23 +3048,23 @@
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="13"/>
       <c r="C113" s="14" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D113" s="14" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E113" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F113" s="14" t="s">
         <v>15</v>
       </c>
       <c r="G113" s="14"/>
       <c r="H113" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I113" s="14" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J113" s="14"/>
       <c r="K113" s="15"/>

</xml_diff>

<commit_message>
Implemented attendance call API
</commit_message>
<xml_diff>
--- a/API List.xlsx
+++ b/API List.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="249">
   <si>
     <t xml:space="preserve">Students</t>
   </si>
@@ -308,6 +308,36 @@
     <t xml:space="preserve">[{session_id, course_name, start_time, duration, series_id}]</t>
   </si>
   <si>
+    <t xml:space="preserve">attendance_call</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/v1.0/attendance_call</t>
+  </si>
+  <si>
+    <t xml:space="preserve">session_id, [student_ids]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">点名</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, take the attendance call for a session</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Courses</t>
   </si>
   <si>
@@ -684,6 +714,9 @@
   </si>
   <si>
     <t xml:space="preserve">/api/v1.0/students_taking_classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authorization: access_token</t>
   </si>
   <si>
     <t xml:space="preserve">class_session_id</t>
@@ -762,7 +795,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -792,6 +825,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Noto Sans CJK SC"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -899,7 +938,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -968,6 +1007,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1007,8 +1054,8 @@
   </sheetPr>
   <dimension ref="B1:K119"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1540,233 +1587,256 @@
       <c r="K23" s="16"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="G25" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I25" s="11" t="s">
+      <c r="I25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J25" s="11" t="s">
+      <c r="J25" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K25" s="12" t="s">
+      <c r="K25" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H26" s="8" t="s">
+      <c r="H26" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="I26" s="8" t="s">
+      <c r="I26" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="J26" s="8"/>
-      <c r="K26" s="18" t="s">
+      <c r="J26" s="6"/>
+      <c r="K26" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="17"/>
-      <c r="C27" s="8" t="s">
+      <c r="B27" s="5"/>
+      <c r="C27" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8" t="s">
+      <c r="E27" s="6"/>
+      <c r="F27" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8" t="s">
+      <c r="G27" s="6"/>
+      <c r="H27" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="I27" s="8" t="s">
+      <c r="I27" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="J27" s="8"/>
-      <c r="K27" s="18"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="17"/>
-      <c r="C28" s="8" t="s">
+      <c r="B28" s="5"/>
+      <c r="C28" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8" t="s">
+      <c r="E28" s="6"/>
+      <c r="F28" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8" t="s">
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="J28" s="8"/>
-      <c r="K28" s="18"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="17"/>
-      <c r="C29" s="8" t="s">
+      <c r="B29" s="5"/>
+      <c r="C29" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8" t="s">
+      <c r="E29" s="6"/>
+      <c r="F29" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8" t="s">
+      <c r="G29" s="6"/>
+      <c r="H29" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="I29" s="8" t="s">
+      <c r="I29" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="J29" s="8"/>
-      <c r="K29" s="18"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="17"/>
-      <c r="C30" s="8" t="s">
+      <c r="B30" s="5"/>
+      <c r="C30" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8" t="s">
+      <c r="G30" s="6"/>
+      <c r="H30" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="I30" s="8" t="s">
+      <c r="I30" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="J30" s="8"/>
-      <c r="K30" s="18" t="s">
+      <c r="J30" s="6"/>
+      <c r="K30" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="G31" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H31" s="14" t="s">
+      <c r="H31" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="I31" s="14" t="s">
+      <c r="I31" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="J31" s="14"/>
-      <c r="K31" s="15"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="G32" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H32" s="14" t="s">
+      <c r="H32" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="I32" s="14" t="s">
+      <c r="I32" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="J32" s="14" t="s">
+      <c r="J32" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="K32" s="15"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="F33" s="16"/>
+      <c r="K32" s="6"/>
+    </row>
+    <row r="33" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I33" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="16"/>
@@ -1775,7 +1845,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="9" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
@@ -1820,62 +1890,62 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G38" s="8"/>
       <c r="H38" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="J38" s="8"/>
-      <c r="K38" s="18"/>
+      <c r="K38" s="20"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="17"/>
+      <c r="B39" s="19"/>
       <c r="C39" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" s="8" t="s">
         <v>101</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>97</v>
       </c>
       <c r="E39" s="8"/>
       <c r="F39" s="8" t="s">
         <v>19</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="H39" s="8"/>
       <c r="I39" s="8" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="J39" s="8"/>
-      <c r="K39" s="18"/>
+      <c r="K39" s="20"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>52</v>
@@ -1886,55 +1956,55 @@
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
       <c r="I40" s="8" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="K40" s="18"/>
+        <v>111</v>
+      </c>
+      <c r="K40" s="20"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="17"/>
+      <c r="B41" s="19"/>
       <c r="C41" s="8" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="J41" s="8"/>
-      <c r="K41" s="18"/>
+      <c r="K41" s="20"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="13"/>
       <c r="C42" s="14" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="14" t="s">
         <v>31</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="H42" s="14"/>
       <c r="I42" s="14" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="J42" s="14"/>
       <c r="K42" s="15" t="s">
@@ -1943,7 +2013,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="9" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
@@ -1988,14 +2058,14 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="E47" s="8"/>
       <c r="F47" s="8" t="s">
@@ -2003,23 +2073,23 @@
       </c>
       <c r="G47" s="8"/>
       <c r="H47" s="8" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="J47" s="8"/>
-      <c r="K47" s="18"/>
+      <c r="K47" s="20"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>52</v>
@@ -2032,25 +2102,25 @@
       </c>
       <c r="H48" s="8"/>
       <c r="I48" s="8" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="J48" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="K48" s="18"/>
+        <v>123</v>
+      </c>
+      <c r="K48" s="20"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>19</v>
@@ -2060,18 +2130,18 @@
       </c>
       <c r="H49" s="8"/>
       <c r="I49" s="8" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="J49" s="8"/>
-      <c r="K49" s="18"/>
+      <c r="K49" s="20"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="17"/>
+      <c r="B50" s="19"/>
       <c r="C50" s="8" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="E50" s="8"/>
       <c r="F50" s="8" t="s">
@@ -2079,21 +2149,21 @@
       </c>
       <c r="G50" s="8"/>
       <c r="H50" s="8" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="J50" s="8"/>
-      <c r="K50" s="18"/>
+      <c r="K50" s="20"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="17"/>
+      <c r="B51" s="19"/>
       <c r="C51" s="8" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="E51" s="8"/>
       <c r="F51" s="8" t="s">
@@ -2102,25 +2172,25 @@
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
       <c r="I51" s="8" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="J51" s="8"/>
-      <c r="K51" s="18" t="s">
+      <c r="K51" s="20" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F52" s="8" t="s">
         <v>15</v>
@@ -2129,26 +2199,26 @@
         <v>53</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="J52" s="8"/>
-      <c r="K52" s="18"/>
+      <c r="K52" s="20"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="17" t="s">
+      <c r="B53" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F53" s="8" t="s">
         <v>15</v>
@@ -2157,23 +2227,23 @@
         <v>53</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="J53" s="8"/>
-      <c r="K53" s="18"/>
+      <c r="K53" s="20"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="E54" s="14"/>
       <c r="F54" s="14" t="s">
@@ -2184,16 +2254,16 @@
       </c>
       <c r="H54" s="14"/>
       <c r="I54" s="14" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="J54" s="14" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="K54" s="15"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="9" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
@@ -2238,12 +2308,12 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="17"/>
+      <c r="B59" s="19"/>
       <c r="C59" s="8" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="8" t="s">
@@ -2251,26 +2321,26 @@
       </c>
       <c r="G59" s="8"/>
       <c r="H59" s="8" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="I59" s="8" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="J59" s="8"/>
-      <c r="K59" s="18"/>
+      <c r="K59" s="20"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="17" t="s">
+      <c r="B60" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="F60" s="8" t="s">
         <v>26</v>
@@ -2279,21 +2349,21 @@
         <v>53</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="I60" s="8" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="J60" s="8"/>
-      <c r="K60" s="18"/>
+      <c r="K60" s="20"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="17"/>
+      <c r="B61" s="19"/>
       <c r="C61" s="8" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>14</v>
@@ -2308,18 +2378,18 @@
         <v>20</v>
       </c>
       <c r="I61" s="8" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="J61" s="8"/>
-      <c r="K61" s="18"/>
+      <c r="K61" s="20"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="17"/>
+      <c r="B62" s="19"/>
       <c r="C62" s="8" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="E62" s="8"/>
       <c r="F62" s="8" t="s">
@@ -2328,18 +2398,18 @@
       <c r="G62" s="8"/>
       <c r="H62" s="8"/>
       <c r="I62" s="8" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="J62" s="8"/>
-      <c r="K62" s="18"/>
+      <c r="K62" s="20"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="13"/>
       <c r="C63" s="14" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="E63" s="14"/>
       <c r="F63" s="14" t="s">
@@ -2348,7 +2418,7 @@
       <c r="G63" s="14"/>
       <c r="H63" s="14"/>
       <c r="I63" s="14" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="J63" s="14"/>
       <c r="K63" s="15" t="s">
@@ -2356,18 +2426,18 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="C66" s="19"/>
-      <c r="D66" s="19"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="19"/>
-      <c r="G66" s="19"/>
-      <c r="H66" s="19"/>
-      <c r="I66" s="19"/>
-      <c r="J66" s="19"/>
-      <c r="K66" s="19"/>
+      <c r="B66" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="C66" s="21"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="21"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="21"/>
+      <c r="H66" s="21"/>
+      <c r="I66" s="21"/>
+      <c r="J66" s="21"/>
+      <c r="K66" s="21"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="10" t="s">
@@ -2402,14 +2472,14 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="17" t="s">
+      <c r="B68" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>36</v>
@@ -2421,21 +2491,21 @@
         <v>53</v>
       </c>
       <c r="H68" s="8" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="I68" s="8" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="J68" s="8"/>
-      <c r="K68" s="18"/>
+      <c r="K68" s="20"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="17"/>
+      <c r="B69" s="19"/>
       <c r="C69" s="8" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E69" s="8"/>
       <c r="F69" s="8" t="s">
@@ -2444,18 +2514,18 @@
       <c r="G69" s="8"/>
       <c r="H69" s="8"/>
       <c r="I69" s="8" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="J69" s="8"/>
-      <c r="K69" s="18"/>
+      <c r="K69" s="20"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="17"/>
+      <c r="B70" s="19"/>
       <c r="C70" s="8" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="E70" s="8"/>
       <c r="F70" s="8" t="s">
@@ -2464,18 +2534,18 @@
       <c r="G70" s="8"/>
       <c r="H70" s="8"/>
       <c r="I70" s="8" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="J70" s="8"/>
-      <c r="K70" s="18"/>
+      <c r="K70" s="20"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="13"/>
       <c r="C71" s="14" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="E71" s="14"/>
       <c r="F71" s="14" t="s">
@@ -2484,7 +2554,7 @@
       <c r="G71" s="14"/>
       <c r="H71" s="14"/>
       <c r="I71" s="14" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="J71" s="14"/>
       <c r="K71" s="15" t="s">
@@ -2493,7 +2563,7 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="9" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C74" s="9"/>
       <c r="D74" s="9"/>
@@ -2538,14 +2608,14 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="17" t="s">
+      <c r="B76" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>14</v>
@@ -2555,24 +2625,24 @@
       </c>
       <c r="G76" s="8"/>
       <c r="H76" s="8" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="I76" s="8" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="J76" s="8"/>
-      <c r="K76" s="18"/>
+      <c r="K76" s="20"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="17"/>
+      <c r="B77" s="19"/>
       <c r="C77" s="8" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F77" s="8" t="s">
         <v>26</v>
@@ -2582,21 +2652,21 @@
       </c>
       <c r="H77" s="8"/>
       <c r="I77" s="8" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="J77" s="8"/>
-      <c r="K77" s="18"/>
+      <c r="K77" s="20"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="17"/>
+      <c r="B78" s="19"/>
       <c r="C78" s="8" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F78" s="8" t="s">
         <v>26</v>
@@ -2606,18 +2676,18 @@
       </c>
       <c r="H78" s="8"/>
       <c r="I78" s="8" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="J78" s="8"/>
-      <c r="K78" s="18"/>
+      <c r="K78" s="20"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="17"/>
+      <c r="B79" s="19"/>
       <c r="C79" s="8" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>14</v>
@@ -2628,20 +2698,20 @@
       <c r="G79" s="8"/>
       <c r="H79" s="8"/>
       <c r="I79" s="8" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="J79" s="8"/>
-      <c r="K79" s="18"/>
+      <c r="K79" s="20"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="17" t="s">
+      <c r="B80" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C80" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D80" s="8" t="s">
         <v>181</v>
-      </c>
-      <c r="D80" s="8" t="s">
-        <v>177</v>
       </c>
       <c r="E80" s="8" t="s">
         <v>14</v>
@@ -2656,20 +2726,20 @@
         <v>92</v>
       </c>
       <c r="I80" s="8" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="J80" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="K80" s="18"/>
+        <v>187</v>
+      </c>
+      <c r="K80" s="20"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="17"/>
+      <c r="B81" s="19"/>
       <c r="C81" s="8" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E81" s="8" t="s">
         <v>14</v>
@@ -2681,21 +2751,21 @@
         <v>53</v>
       </c>
       <c r="H81" s="8" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="I81" s="8" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="J81" s="8"/>
-      <c r="K81" s="18"/>
+      <c r="K81" s="20"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="17"/>
+      <c r="B82" s="19"/>
       <c r="C82" s="8" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="E82" s="8" t="s">
         <v>14</v>
@@ -2708,18 +2778,18 @@
       </c>
       <c r="H82" s="8"/>
       <c r="I82" s="8" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="J82" s="8"/>
-      <c r="K82" s="18"/>
+      <c r="K82" s="20"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="13"/>
       <c r="C83" s="14" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="E83" s="14"/>
       <c r="F83" s="14" t="s">
@@ -2728,7 +2798,7 @@
       <c r="G83" s="14"/>
       <c r="H83" s="14"/>
       <c r="I83" s="14" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="J83" s="14"/>
       <c r="K83" s="15" t="s">
@@ -2737,7 +2807,7 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="9" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="C86" s="9"/>
       <c r="D86" s="9"/>
@@ -2782,12 +2852,12 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="17"/>
+      <c r="B88" s="19"/>
       <c r="C88" s="8" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="E88" s="8"/>
       <c r="F88" s="8" t="s">
@@ -2795,21 +2865,21 @@
       </c>
       <c r="G88" s="8"/>
       <c r="H88" s="8" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="I88" s="8" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="J88" s="8"/>
-      <c r="K88" s="18"/>
+      <c r="K88" s="20"/>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="17"/>
+      <c r="B89" s="19"/>
       <c r="C89" s="8" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="E89" s="8"/>
       <c r="F89" s="8" t="s">
@@ -2817,21 +2887,21 @@
       </c>
       <c r="G89" s="8"/>
       <c r="H89" s="8" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="I89" s="8" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="J89" s="8"/>
-      <c r="K89" s="18"/>
+      <c r="K89" s="20"/>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="17"/>
+      <c r="B90" s="19"/>
       <c r="C90" s="8" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E90" s="8"/>
       <c r="F90" s="8" t="s">
@@ -2842,51 +2912,51 @@
       </c>
       <c r="H90" s="8"/>
       <c r="I90" s="8" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="J90" s="8"/>
-      <c r="K90" s="18"/>
+      <c r="K90" s="20"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="17"/>
+      <c r="B91" s="19"/>
       <c r="C91" s="8" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="E91" s="8"/>
       <c r="F91" s="8" t="s">
         <v>19</v>
       </c>
       <c r="G91" s="8" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="H91" s="8"/>
       <c r="I91" s="8" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="J91" s="8"/>
-      <c r="K91" s="18"/>
+      <c r="K91" s="20"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="13"/>
       <c r="C92" s="14" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="D92" s="14" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="E92" s="14"/>
       <c r="F92" s="14" t="s">
         <v>31</v>
       </c>
       <c r="G92" s="14" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="H92" s="14"/>
       <c r="I92" s="14" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="J92" s="14"/>
       <c r="K92" s="15" t="s">
@@ -2895,7 +2965,7 @@
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="9" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C95" s="9"/>
       <c r="D95" s="9"/>
@@ -2940,14 +3010,14 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="17" t="s">
+      <c r="B97" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="E97" s="8"/>
       <c r="F97" s="8" t="s">
@@ -2955,21 +3025,21 @@
       </c>
       <c r="G97" s="8"/>
       <c r="H97" s="8" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="I97" s="8" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J97" s="8"/>
-      <c r="K97" s="18"/>
+      <c r="K97" s="20"/>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="17"/>
+      <c r="B98" s="19"/>
       <c r="C98" s="8" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="E98" s="8"/>
       <c r="F98" s="8" t="s">
@@ -2977,18 +3047,18 @@
       </c>
       <c r="G98" s="8"/>
       <c r="H98" s="8" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="I98" s="8" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="J98" s="8"/>
-      <c r="K98" s="18"/>
+      <c r="K98" s="20"/>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="17"/>
+      <c r="B99" s="19"/>
       <c r="C99" s="8" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D99" s="8"/>
       <c r="E99" s="8"/>
@@ -3000,40 +3070,44 @@
         <v>20</v>
       </c>
       <c r="I99" s="8" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="J99" s="8"/>
-      <c r="K99" s="18"/>
+      <c r="K99" s="20"/>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="17"/>
+      <c r="B100" s="19" t="s">
+        <v>11</v>
+      </c>
       <c r="C100" s="8" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="E100" s="8"/>
       <c r="F100" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G100" s="8"/>
+        <v>15</v>
+      </c>
+      <c r="G100" s="8" t="s">
+        <v>225</v>
+      </c>
       <c r="H100" s="8" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="I100" s="8" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="J100" s="8"/>
-      <c r="K100" s="18"/>
+      <c r="K100" s="20"/>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="13"/>
       <c r="C101" s="14" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="E101" s="14"/>
       <c r="F101" s="14" t="s">
@@ -3042,7 +3116,7 @@
       <c r="G101" s="14"/>
       <c r="H101" s="14"/>
       <c r="I101" s="14" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="J101" s="14"/>
       <c r="K101" s="15" t="s">
@@ -3096,14 +3170,14 @@
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B106" s="17" t="s">
+      <c r="B106" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="E106" s="8"/>
       <c r="F106" s="8" t="s">
@@ -3111,47 +3185,47 @@
       </c>
       <c r="G106" s="8"/>
       <c r="H106" s="8" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="I106" s="8" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="J106" s="8"/>
-      <c r="K106" s="18"/>
+      <c r="K106" s="20"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="17" t="s">
+      <c r="B107" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="E107" s="8"/>
       <c r="F107" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G107" s="8" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="H107" s="8"/>
       <c r="I107" s="8" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="J107" s="8"/>
-      <c r="K107" s="18"/>
+      <c r="K107" s="20"/>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="17" t="s">
+      <c r="B108" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="E108" s="8"/>
       <c r="F108" s="8" t="s">
@@ -3162,20 +3236,20 @@
       </c>
       <c r="H108" s="8"/>
       <c r="I108" s="8" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="J108" s="8"/>
-      <c r="K108" s="18"/>
+      <c r="K108" s="20"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C109" s="14" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="D109" s="14" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="E109" s="14"/>
       <c r="F109" s="14" t="s">
@@ -3183,10 +3257,10 @@
       </c>
       <c r="G109" s="14"/>
       <c r="H109" s="14" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="I109" s="14" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="J109" s="14"/>
       <c r="K109" s="15"/>
@@ -3228,18 +3302,18 @@
       <c r="K112" s="8"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B115" s="20"/>
-      <c r="C115" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="D115" s="21"/>
-      <c r="E115" s="21"/>
-      <c r="F115" s="21"/>
-      <c r="G115" s="21"/>
-      <c r="H115" s="21"/>
-      <c r="I115" s="21"/>
-      <c r="J115" s="21"/>
-      <c r="K115" s="21"/>
+      <c r="B115" s="22"/>
+      <c r="C115" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="D115" s="23"/>
+      <c r="E115" s="23"/>
+      <c r="F115" s="23"/>
+      <c r="G115" s="23"/>
+      <c r="H115" s="23"/>
+      <c r="I115" s="23"/>
+      <c r="J115" s="23"/>
+      <c r="K115" s="23"/>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="10" t="s">
@@ -3276,13 +3350,13 @@
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="13"/>
       <c r="C117" s="14" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="D117" s="14" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="E117" s="14" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F117" s="14" t="s">
         <v>15</v>
@@ -3292,7 +3366,7 @@
         <v>77</v>
       </c>
       <c r="I117" s="14" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="J117" s="14"/>
       <c r="K117" s="15"/>

</xml_diff>

<commit_message>
Changed models naming, implemented get admins and get teachers
</commit_message>
<xml_diff>
--- a/API List.xlsx
+++ b/API List.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="250">
   <si>
     <t xml:space="preserve">Students</t>
   </si>
@@ -266,7 +266,13 @@
     <t xml:space="preserve">/api/v1.0/teachers</t>
   </si>
   <si>
+    <t xml:space="preserve">Principle</t>
+  </si>
+  <si>
     <t xml:space="preserve">Get a list of all teachers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{teacher_id, realName}]</t>
   </si>
   <si>
     <t xml:space="preserve">update_teacher</t>
@@ -323,6 +329,7 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">点名</t>
     </r>
@@ -489,9 +496,6 @@
   </si>
   <si>
     <t xml:space="preserve">update_course_credit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Principle</t>
   </si>
   <si>
     <t xml:space="preserve">Update a course_credit's information or add a course_credit record</t>
@@ -831,6 +835,7 @@
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1054,8 +1059,8 @@
   </sheetPr>
   <dimension ref="B1:K119"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1692,22 +1697,28 @@
       <c r="D28" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E28" s="6"/>
+      <c r="E28" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="F28" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G28" s="6"/>
+      <c r="G28" s="6" t="s">
+        <v>45</v>
+      </c>
       <c r="H28" s="6"/>
       <c r="I28" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="J28" s="6"/>
+        <v>82</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="K28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="5"/>
       <c r="C29" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>74</v>
@@ -1718,10 +1729,10 @@
       </c>
       <c r="G29" s="6"/>
       <c r="H29" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
@@ -1729,7 +1740,7 @@
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="5"/>
       <c r="C30" s="6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>74</v>
@@ -1745,7 +1756,7 @@
         <v>77</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="J30" s="6"/>
       <c r="K30" s="6" t="s">
@@ -1757,10 +1768,10 @@
         <v>11</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>30</v>
@@ -1775,7 +1786,7 @@
         <v>77</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
@@ -1785,10 +1796,10 @@
         <v>11</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>14</v>
@@ -1800,13 +1811,13 @@
         <v>45</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K32" s="6"/>
     </row>
@@ -1815,10 +1826,10 @@
         <v>11</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>14</v>
@@ -1830,10 +1841,10 @@
         <v>45</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I33" s="18" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
@@ -1845,7 +1856,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="9" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
@@ -1894,23 +1905,23 @@
         <v>11</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G38" s="8"/>
       <c r="H38" s="8" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J38" s="8"/>
       <c r="K38" s="20"/>
@@ -1918,21 +1929,21 @@
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="19"/>
       <c r="C39" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E39" s="8"/>
       <c r="F39" s="8" t="s">
         <v>19</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H39" s="8"/>
       <c r="I39" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="J39" s="8"/>
       <c r="K39" s="20"/>
@@ -1942,10 +1953,10 @@
         <v>11</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>52</v>
@@ -1956,33 +1967,33 @@
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
       <c r="I40" s="8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="K40" s="20"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="19"/>
       <c r="C41" s="8" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="J41" s="8"/>
       <c r="K41" s="20"/>
@@ -1990,21 +2001,21 @@
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="13"/>
       <c r="C42" s="14" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="14" t="s">
         <v>31</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H42" s="14"/>
       <c r="I42" s="14" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="J42" s="14"/>
       <c r="K42" s="15" t="s">
@@ -2013,7 +2024,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="9" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
@@ -2062,10 +2073,10 @@
         <v>11</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E47" s="8"/>
       <c r="F47" s="8" t="s">
@@ -2073,10 +2084,10 @@
       </c>
       <c r="G47" s="8"/>
       <c r="H47" s="8" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J47" s="8"/>
       <c r="K47" s="20"/>
@@ -2086,10 +2097,10 @@
         <v>11</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>52</v>
@@ -2102,10 +2113,10 @@
       </c>
       <c r="H48" s="8"/>
       <c r="I48" s="8" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="J48" s="8" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="K48" s="20"/>
     </row>
@@ -2114,13 +2125,13 @@
         <v>11</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>19</v>
@@ -2130,7 +2141,7 @@
       </c>
       <c r="H49" s="8"/>
       <c r="I49" s="8" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="J49" s="8"/>
       <c r="K49" s="20"/>
@@ -2138,10 +2149,10 @@
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="19"/>
       <c r="C50" s="8" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E50" s="8"/>
       <c r="F50" s="8" t="s">
@@ -2149,10 +2160,10 @@
       </c>
       <c r="G50" s="8"/>
       <c r="H50" s="8" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="J50" s="8"/>
       <c r="K50" s="20"/>
@@ -2160,10 +2171,10 @@
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="19"/>
       <c r="C51" s="8" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E51" s="8"/>
       <c r="F51" s="8" t="s">
@@ -2172,7 +2183,7 @@
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
       <c r="I51" s="8" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="J51" s="8"/>
       <c r="K51" s="20" t="s">
@@ -2184,13 +2195,13 @@
         <v>11</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F52" s="8" t="s">
         <v>15</v>
@@ -2199,10 +2210,10 @@
         <v>53</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="J52" s="8"/>
       <c r="K52" s="20"/>
@@ -2212,13 +2223,13 @@
         <v>11</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F53" s="8" t="s">
         <v>15</v>
@@ -2227,10 +2238,10 @@
         <v>53</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="J53" s="8"/>
       <c r="K53" s="20"/>
@@ -2240,10 +2251,10 @@
         <v>11</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E54" s="14"/>
       <c r="F54" s="14" t="s">
@@ -2254,16 +2265,16 @@
       </c>
       <c r="H54" s="14"/>
       <c r="I54" s="14" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="J54" s="14" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="K54" s="15"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="9" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
@@ -2310,10 +2321,10 @@
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="19"/>
       <c r="C59" s="8" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="8" t="s">
@@ -2321,10 +2332,10 @@
       </c>
       <c r="G59" s="8"/>
       <c r="H59" s="8" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I59" s="8" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="J59" s="8"/>
       <c r="K59" s="20"/>
@@ -2334,13 +2345,13 @@
         <v>11</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>150</v>
+        <v>81</v>
       </c>
       <c r="F60" s="8" t="s">
         <v>26</v>
@@ -2349,10 +2360,10 @@
         <v>53</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I60" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J60" s="8"/>
       <c r="K60" s="20"/>
@@ -2360,10 +2371,10 @@
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="19"/>
       <c r="C61" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>14</v>
@@ -2378,7 +2389,7 @@
         <v>20</v>
       </c>
       <c r="I61" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="J61" s="8"/>
       <c r="K61" s="20"/>
@@ -2386,10 +2397,10 @@
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="19"/>
       <c r="C62" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E62" s="8"/>
       <c r="F62" s="8" t="s">
@@ -2398,7 +2409,7 @@
       <c r="G62" s="8"/>
       <c r="H62" s="8"/>
       <c r="I62" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="J62" s="8"/>
       <c r="K62" s="20"/>
@@ -2406,10 +2417,10 @@
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="13"/>
       <c r="C63" s="14" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E63" s="14"/>
       <c r="F63" s="14" t="s">
@@ -2418,7 +2429,7 @@
       <c r="G63" s="14"/>
       <c r="H63" s="14"/>
       <c r="I63" s="14" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="J63" s="14"/>
       <c r="K63" s="15" t="s">
@@ -2427,7 +2438,7 @@
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="21" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C66" s="21"/>
       <c r="D66" s="21"/>
@@ -2476,10 +2487,10 @@
         <v>11</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>36</v>
@@ -2491,10 +2502,10 @@
         <v>53</v>
       </c>
       <c r="H68" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="I68" s="8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="J68" s="8"/>
       <c r="K68" s="20"/>
@@ -2502,10 +2513,10 @@
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="19"/>
       <c r="C69" s="8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E69" s="8"/>
       <c r="F69" s="8" t="s">
@@ -2514,7 +2525,7 @@
       <c r="G69" s="8"/>
       <c r="H69" s="8"/>
       <c r="I69" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="J69" s="8"/>
       <c r="K69" s="20"/>
@@ -2522,10 +2533,10 @@
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="19"/>
       <c r="C70" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E70" s="8"/>
       <c r="F70" s="8" t="s">
@@ -2534,7 +2545,7 @@
       <c r="G70" s="8"/>
       <c r="H70" s="8"/>
       <c r="I70" s="8" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="J70" s="8"/>
       <c r="K70" s="20"/>
@@ -2542,10 +2553,10 @@
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="13"/>
       <c r="C71" s="14" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E71" s="14"/>
       <c r="F71" s="14" t="s">
@@ -2554,7 +2565,7 @@
       <c r="G71" s="14"/>
       <c r="H71" s="14"/>
       <c r="I71" s="14" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J71" s="14"/>
       <c r="K71" s="15" t="s">
@@ -2563,7 +2574,7 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C74" s="9"/>
       <c r="D74" s="9"/>
@@ -2612,10 +2623,10 @@
         <v>11</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>14</v>
@@ -2625,10 +2636,10 @@
       </c>
       <c r="G76" s="8"/>
       <c r="H76" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I76" s="8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J76" s="8"/>
       <c r="K76" s="20"/>
@@ -2636,13 +2647,13 @@
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="19"/>
       <c r="C77" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F77" s="8" t="s">
         <v>26</v>
@@ -2652,7 +2663,7 @@
       </c>
       <c r="H77" s="8"/>
       <c r="I77" s="8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J77" s="8"/>
       <c r="K77" s="20"/>
@@ -2660,13 +2671,13 @@
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="19"/>
       <c r="C78" s="8" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F78" s="8" t="s">
         <v>26</v>
@@ -2676,7 +2687,7 @@
       </c>
       <c r="H78" s="8"/>
       <c r="I78" s="8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="J78" s="8"/>
       <c r="K78" s="20"/>
@@ -2684,10 +2695,10 @@
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="19"/>
       <c r="C79" s="8" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>14</v>
@@ -2698,7 +2709,7 @@
       <c r="G79" s="8"/>
       <c r="H79" s="8"/>
       <c r="I79" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="J79" s="8"/>
       <c r="K79" s="20"/>
@@ -2708,10 +2719,10 @@
         <v>11</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E80" s="8" t="s">
         <v>14</v>
@@ -2723,23 +2734,23 @@
         <v>53</v>
       </c>
       <c r="H80" s="8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I80" s="8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J80" s="8" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K80" s="20"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="19"/>
       <c r="C81" s="8" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E81" s="8" t="s">
         <v>14</v>
@@ -2751,10 +2762,10 @@
         <v>53</v>
       </c>
       <c r="H81" s="8" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="I81" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J81" s="8"/>
       <c r="K81" s="20"/>
@@ -2762,10 +2773,10 @@
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="19"/>
       <c r="C82" s="8" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E82" s="8" t="s">
         <v>14</v>
@@ -2778,7 +2789,7 @@
       </c>
       <c r="H82" s="8"/>
       <c r="I82" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="J82" s="8"/>
       <c r="K82" s="20"/>
@@ -2786,10 +2797,10 @@
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="13"/>
       <c r="C83" s="14" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E83" s="14"/>
       <c r="F83" s="14" t="s">
@@ -2798,7 +2809,7 @@
       <c r="G83" s="14"/>
       <c r="H83" s="14"/>
       <c r="I83" s="14" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="J83" s="14"/>
       <c r="K83" s="15" t="s">
@@ -2807,7 +2818,7 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="9" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C86" s="9"/>
       <c r="D86" s="9"/>
@@ -2854,10 +2865,10 @@
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="19"/>
       <c r="C88" s="8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D88" s="8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E88" s="8"/>
       <c r="F88" s="8" t="s">
@@ -2865,10 +2876,10 @@
       </c>
       <c r="G88" s="8"/>
       <c r="H88" s="8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I88" s="8" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J88" s="8"/>
       <c r="K88" s="20"/>
@@ -2876,10 +2887,10 @@
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="19"/>
       <c r="C89" s="8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E89" s="8"/>
       <c r="F89" s="8" t="s">
@@ -2887,10 +2898,10 @@
       </c>
       <c r="G89" s="8"/>
       <c r="H89" s="8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I89" s="8" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="J89" s="8"/>
       <c r="K89" s="20"/>
@@ -2898,10 +2909,10 @@
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="19"/>
       <c r="C90" s="8" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E90" s="8"/>
       <c r="F90" s="8" t="s">
@@ -2912,7 +2923,7 @@
       </c>
       <c r="H90" s="8"/>
       <c r="I90" s="8" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J90" s="8"/>
       <c r="K90" s="20"/>
@@ -2920,21 +2931,21 @@
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="19"/>
       <c r="C91" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E91" s="8"/>
       <c r="F91" s="8" t="s">
         <v>19</v>
       </c>
       <c r="G91" s="8" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H91" s="8"/>
       <c r="I91" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J91" s="8"/>
       <c r="K91" s="20"/>
@@ -2942,21 +2953,21 @@
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="13"/>
       <c r="C92" s="14" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D92" s="14" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E92" s="14"/>
       <c r="F92" s="14" t="s">
         <v>31</v>
       </c>
       <c r="G92" s="14" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H92" s="14"/>
       <c r="I92" s="14" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="J92" s="14"/>
       <c r="K92" s="15" t="s">
@@ -2965,7 +2976,7 @@
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="9" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C95" s="9"/>
       <c r="D95" s="9"/>
@@ -3014,10 +3025,10 @@
         <v>11</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E97" s="8"/>
       <c r="F97" s="8" t="s">
@@ -3025,10 +3036,10 @@
       </c>
       <c r="G97" s="8"/>
       <c r="H97" s="8" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="I97" s="8" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="J97" s="8"/>
       <c r="K97" s="20"/>
@@ -3036,10 +3047,10 @@
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="19"/>
       <c r="C98" s="8" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E98" s="8"/>
       <c r="F98" s="8" t="s">
@@ -3047,10 +3058,10 @@
       </c>
       <c r="G98" s="8"/>
       <c r="H98" s="8" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I98" s="8" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="J98" s="8"/>
       <c r="K98" s="20"/>
@@ -3058,7 +3069,7 @@
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="19"/>
       <c r="C99" s="8" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D99" s="8"/>
       <c r="E99" s="8"/>
@@ -3070,7 +3081,7 @@
         <v>20</v>
       </c>
       <c r="I99" s="8" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="J99" s="8"/>
       <c r="K99" s="20"/>
@@ -3080,23 +3091,23 @@
         <v>11</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E100" s="8"/>
       <c r="F100" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G100" s="8" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="H100" s="8" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="I100" s="8" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="J100" s="8"/>
       <c r="K100" s="20"/>
@@ -3104,10 +3115,10 @@
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="13"/>
       <c r="C101" s="14" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E101" s="14"/>
       <c r="F101" s="14" t="s">
@@ -3116,7 +3127,7 @@
       <c r="G101" s="14"/>
       <c r="H101" s="14"/>
       <c r="I101" s="14" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J101" s="14"/>
       <c r="K101" s="15" t="s">
@@ -3174,10 +3185,10 @@
         <v>11</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E106" s="8"/>
       <c r="F106" s="8" t="s">
@@ -3185,10 +3196,10 @@
       </c>
       <c r="G106" s="8"/>
       <c r="H106" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I106" s="8" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="J106" s="8"/>
       <c r="K106" s="20"/>
@@ -3198,21 +3209,21 @@
         <v>11</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E107" s="8"/>
       <c r="F107" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G107" s="8" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H107" s="8"/>
       <c r="I107" s="8" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="J107" s="8"/>
       <c r="K107" s="20"/>
@@ -3222,10 +3233,10 @@
         <v>11</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E108" s="8"/>
       <c r="F108" s="8" t="s">
@@ -3236,7 +3247,7 @@
       </c>
       <c r="H108" s="8"/>
       <c r="I108" s="8" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="J108" s="8"/>
       <c r="K108" s="20"/>
@@ -3246,10 +3257,10 @@
         <v>11</v>
       </c>
       <c r="C109" s="14" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D109" s="14" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E109" s="14"/>
       <c r="F109" s="14" t="s">
@@ -3257,10 +3268,10 @@
       </c>
       <c r="G109" s="14"/>
       <c r="H109" s="14" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="I109" s="14" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="J109" s="14"/>
       <c r="K109" s="15"/>
@@ -3304,7 +3315,7 @@
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="22"/>
       <c r="C115" s="23" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D115" s="23"/>
       <c r="E115" s="23"/>
@@ -3350,13 +3361,13 @@
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B117" s="13"/>
       <c r="C117" s="14" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D117" s="14" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E117" s="14" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F117" s="14" t="s">
         <v>15</v>
@@ -3366,7 +3377,7 @@
         <v>77</v>
       </c>
       <c r="I117" s="14" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="J117" s="14"/>
       <c r="K117" s="15"/>

</xml_diff>

<commit_message>
updated api excel list
</commit_message>
<xml_diff>
--- a/API List.xlsx
+++ b/API List.xlsx
@@ -21,9 +21,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="250">
-  <si>
-    <t xml:space="preserve">Students</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="269">
+  <si>
+    <t xml:space="preserve">Students*</t>
   </si>
   <si>
     <t xml:space="preserve">Implemented</t>
@@ -170,7 +170,16 @@
     <t xml:space="preserve">[{attended, course_name, duration, series_id, session_id, start_time}]</t>
   </si>
   <si>
-    <t xml:space="preserve">Parents</t>
+    <t xml:space="preserve">get_student_parents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authorization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get a list of parents for the student</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parents*</t>
   </si>
   <si>
     <t xml:space="preserve">add_parent</t>
@@ -182,9 +191,6 @@
     <t xml:space="preserve">everybody</t>
   </si>
   <si>
-    <t xml:space="preserve">Authorization</t>
-  </si>
-  <si>
     <t xml:space="preserve">realName, phone, gender, language, province, city, avatar</t>
   </si>
   <si>
@@ -206,7 +212,7 @@
     <t xml:space="preserve">/api/v1.0/validate_parent</t>
   </si>
   <si>
-    <t xml:space="preserve">parent_id</t>
+    <t xml:space="preserve">parent_id, decision</t>
   </si>
   <si>
     <t xml:space="preserve">Validate a registered parent.</t>
@@ -239,7 +245,7 @@
     <t xml:space="preserve">{“successfully binded”} or {“modified relationship from # to #”}</t>
   </si>
   <si>
-    <t xml:space="preserve">Teachers</t>
+    <t xml:space="preserve">Teachers*</t>
   </si>
   <si>
     <t xml:space="preserve">add_teacher</t>
@@ -266,13 +272,13 @@
     <t xml:space="preserve">/api/v1.0/teachers</t>
   </si>
   <si>
-    <t xml:space="preserve">Principle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get a list of all teachers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[{teacher_id, realName}]</t>
+    <t xml:space="preserve">Admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get a list of all undeleted teachers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[{validate_info}]</t>
   </si>
   <si>
     <t xml:space="preserve">update_teacher</t>
@@ -345,7 +351,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Courses</t>
+    <t xml:space="preserve">Courses*</t>
   </si>
   <si>
     <t xml:space="preserve">add_course</t>
@@ -396,7 +402,7 @@
     <t xml:space="preserve">Delete one course</t>
   </si>
   <si>
-    <t xml:space="preserve">Users</t>
+    <t xml:space="preserve">Users*</t>
   </si>
   <si>
     <t xml:space="preserve">add_user</t>
@@ -426,9 +432,6 @@
     <t xml:space="preserve">/api/v1.0/unvalidated_users</t>
   </si>
   <si>
-    <t xml:space="preserve">Admin</t>
-  </si>
-  <si>
     <t xml:space="preserve">Get a list of all unapproved users</t>
   </si>
   <si>
@@ -462,7 +465,7 @@
     <t xml:space="preserve">/api/v1.0/validate_user</t>
   </si>
   <si>
-    <t xml:space="preserve">user_id</t>
+    <t xml:space="preserve">user_id, decision</t>
   </si>
   <si>
     <t xml:space="preserve">Validate a registered user, add the approver info and approve time</t>
@@ -480,9 +483,54 @@
     <t xml:space="preserve">user_role, validated</t>
   </si>
   <si>
+    <t xml:space="preserve">add_admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/v1.0/add_admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avatar, phone, gender, real_name, language, province, city, register_time, nick_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register one admin to the DB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This api will change the validation status of an user to WAITING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate_admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/v1.0/validate_admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Super</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin_id, decision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This API validates an admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This api changes the validation status of an admin to one of the three status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get_admins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/v1.0/get_admins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This API returns a list of admins, not including the revoked ones.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Course Credit</t>
   </si>
   <si>
+    <t xml:space="preserve">File</t>
+  </si>
+  <si>
     <t xml:space="preserve">add_course_credit</t>
   </si>
   <si>
@@ -498,9 +546,15 @@
     <t xml:space="preserve">update_course_credit</t>
   </si>
   <si>
+    <t xml:space="preserve">Principle</t>
+  </si>
+  <si>
     <t xml:space="preserve">Update a course_credit's information or add a course_credit record</t>
   </si>
   <si>
+    <t xml:space="preserve">course</t>
+  </si>
+  <si>
     <t xml:space="preserve">get_student_course_credits</t>
   </si>
   <si>
@@ -528,7 +582,7 @@
     <t xml:space="preserve">Parent Hood</t>
   </si>
   <si>
-    <t xml:space="preserve">add_parent_hood</t>
+    <t xml:space="preserve">update_parent_hood</t>
   </si>
   <si>
     <t xml:space="preserve">/api/v1.0/parent_hood</t>
@@ -538,6 +592,9 @@
   </si>
   <si>
     <t xml:space="preserve">Update or create a parent_hood's information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">student</t>
   </si>
   <si>
     <t xml:space="preserve">get_student_parent_hoods</t>
@@ -846,7 +903,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -901,13 +958,6 @@
       <right style="hair"/>
       <top/>
       <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -1028,15 +1078,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1057,10 +1107,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:K119"/>
+  <dimension ref="B1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B91" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1347,15 +1397,33 @@
       <c r="K11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
+      <c r="B12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="K12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1384,7 +1452,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="9" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -1433,29 +1501,29 @@
         <v>11</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F17" s="14" t="s">
         <v>15</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="J17" s="14"/>
       <c r="K17" s="15" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1464,7 +1532,7 @@
         <v>22</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>36</v>
@@ -1473,11 +1541,11 @@
         <v>19</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H18" s="14"/>
       <c r="I18" s="14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J18" s="14"/>
       <c r="K18" s="15"/>
@@ -1487,10 +1555,10 @@
         <v>11</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>14</v>
@@ -1502,10 +1570,10 @@
         <v>45</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J19" s="14"/>
       <c r="K19" s="15"/>
@@ -1515,10 +1583,10 @@
         <v>11</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>14</v>
@@ -1531,22 +1599,20 @@
       </c>
       <c r="H20" s="14"/>
       <c r="I20" s="14" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K20" s="15"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="13" t="s">
-        <v>11</v>
-      </c>
+      <c r="B21" s="13"/>
       <c r="C21" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>36</v>
@@ -1558,13 +1624,13 @@
         <v>45</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K21" s="15"/>
     </row>
@@ -1593,7 +1659,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="17" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -1642,38 +1708,38 @@
         <v>11</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>15</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="J26" s="6"/>
       <c r="K26" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="5"/>
       <c r="C27" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>74</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="6" t="s">
@@ -1681,24 +1747,26 @@
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="5"/>
+      <c r="B28" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="C28" s="6" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>19</v>
@@ -1708,20 +1776,20 @@
       </c>
       <c r="H28" s="6"/>
       <c r="I28" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="5"/>
       <c r="C29" s="6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6" t="s">
@@ -1729,10 +1797,10 @@
       </c>
       <c r="G29" s="6"/>
       <c r="H29" s="6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
@@ -1740,10 +1808,10 @@
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="5"/>
       <c r="C30" s="6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>30</v>
@@ -1753,10 +1821,10 @@
       </c>
       <c r="G30" s="6"/>
       <c r="H30" s="6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J30" s="6"/>
       <c r="K30" s="6" t="s">
@@ -1768,10 +1836,10 @@
         <v>11</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>30</v>
@@ -1783,10 +1851,10 @@
         <v>45</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
@@ -1796,10 +1864,10 @@
         <v>11</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>14</v>
@@ -1811,13 +1879,13 @@
         <v>45</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="K32" s="6"/>
     </row>
@@ -1826,10 +1894,10 @@
         <v>11</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>14</v>
@@ -1841,10 +1909,10 @@
         <v>45</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I33" s="18" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J33" s="6"/>
       <c r="K33" s="6"/>
@@ -1856,7 +1924,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
@@ -1905,23 +1973,23 @@
         <v>11</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G38" s="8"/>
       <c r="H38" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J38" s="8"/>
       <c r="K38" s="20"/>
@@ -1929,21 +1997,21 @@
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="19"/>
       <c r="C39" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E39" s="8"/>
       <c r="F39" s="8" t="s">
         <v>19</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H39" s="8"/>
       <c r="I39" s="8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="J39" s="8"/>
       <c r="K39" s="20"/>
@@ -1953,13 +2021,13 @@
         <v>11</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>19</v>
@@ -1967,33 +2035,33 @@
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
       <c r="I40" s="8" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K40" s="20"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="19"/>
       <c r="C41" s="8" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="J41" s="8"/>
       <c r="K41" s="20"/>
@@ -2001,21 +2069,21 @@
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="13"/>
       <c r="C42" s="14" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E42" s="14"/>
       <c r="F42" s="14" t="s">
         <v>31</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H42" s="14"/>
       <c r="I42" s="14" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="J42" s="14"/>
       <c r="K42" s="15" t="s">
@@ -2024,7 +2092,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="9" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
@@ -2073,10 +2141,10 @@
         <v>11</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E47" s="8"/>
       <c r="F47" s="8" t="s">
@@ -2084,10 +2152,10 @@
       </c>
       <c r="G47" s="8"/>
       <c r="H47" s="8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="J47" s="8"/>
       <c r="K47" s="20"/>
@@ -2097,26 +2165,26 @@
         <v>11</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F48" s="8" t="s">
         <v>19</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H48" s="8"/>
       <c r="I48" s="8" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="J48" s="8" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="K48" s="20"/>
     </row>
@@ -2125,23 +2193,23 @@
         <v>11</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>128</v>
+        <v>83</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>19</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H49" s="8"/>
       <c r="I49" s="8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J49" s="8"/>
       <c r="K49" s="20"/>
@@ -2149,10 +2217,10 @@
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="19"/>
       <c r="C50" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E50" s="8"/>
       <c r="F50" s="8" t="s">
@@ -2160,10 +2228,10 @@
       </c>
       <c r="G50" s="8"/>
       <c r="H50" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J50" s="8"/>
       <c r="K50" s="20"/>
@@ -2171,10 +2239,10 @@
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="19"/>
       <c r="C51" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E51" s="8"/>
       <c r="F51" s="8" t="s">
@@ -2183,7 +2251,7 @@
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
       <c r="I51" s="8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J51" s="8"/>
       <c r="K51" s="20" t="s">
@@ -2195,25 +2263,25 @@
         <v>11</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>128</v>
+        <v>83</v>
       </c>
       <c r="F52" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="J52" s="8"/>
       <c r="K52" s="20"/>
@@ -2223,25 +2291,25 @@
         <v>11</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>128</v>
+        <v>83</v>
       </c>
       <c r="F53" s="8" t="s">
         <v>15</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J53" s="8"/>
       <c r="K53" s="20"/>
@@ -2251,521 +2319,552 @@
         <v>11</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E54" s="14"/>
       <c r="F54" s="14" t="s">
         <v>19</v>
       </c>
       <c r="G54" s="14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H54" s="14"/>
       <c r="I54" s="14" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J54" s="14" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="K54" s="15"/>
     </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F55" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G55" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H55" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="I55" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="J55" s="14"/>
+      <c r="K55" s="15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="E56" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="F56" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G56" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H56" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="I56" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="J56" s="14"/>
+      <c r="K56" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="9"/>
-      <c r="K57" s="9"/>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="10" t="s">
+      <c r="B57" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="F57" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G57" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="J57" s="14"/>
+      <c r="K57" s="15"/>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9"/>
+      <c r="K60" s="9"/>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="C61" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D58" s="11" t="s">
+      <c r="D61" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E58" s="11" t="s">
+      <c r="E61" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F58" s="11" t="s">
+      <c r="F61" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G58" s="11" t="s">
+      <c r="G61" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H58" s="11" t="s">
+      <c r="H61" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I58" s="11" t="s">
+      <c r="I61" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J58" s="11" t="s">
+      <c r="J61" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K58" s="12" t="s">
+      <c r="K61" s="12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="19"/>
-      <c r="C59" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G59" s="8"/>
-      <c r="H59" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="I59" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="J59" s="8"/>
-      <c r="K59" s="20"/>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="F60" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G60" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H60" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="I60" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="J60" s="8"/>
-      <c r="K60" s="20"/>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="19"/>
-      <c r="C61" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="E61" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F61" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G61" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H61" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I61" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="J61" s="8"/>
-      <c r="K61" s="20"/>
+      <c r="L61" s="0" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="19"/>
       <c r="C62" s="8" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="E62" s="8"/>
       <c r="F62" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G62" s="8"/>
-      <c r="H62" s="8"/>
+      <c r="H62" s="8" t="s">
+        <v>165</v>
+      </c>
       <c r="I62" s="8" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="J62" s="8"/>
       <c r="K62" s="20"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="13"/>
-      <c r="C63" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="D63" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14" t="s">
+      <c r="B63" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G63" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H63" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="I63" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J63" s="8"/>
+      <c r="K63" s="20"/>
+      <c r="L63" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="19"/>
+      <c r="C64" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G64" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H64" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I64" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="J64" s="8"/>
+      <c r="K64" s="20"/>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="19"/>
+      <c r="C65" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G65" s="8"/>
+      <c r="H65" s="8"/>
+      <c r="I65" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="J65" s="8"/>
+      <c r="K65" s="20"/>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="13"/>
+      <c r="C66" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="D66" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="J63" s="14"/>
-      <c r="K63" s="15" t="s">
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="J66" s="14"/>
+      <c r="K66" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="C66" s="21"/>
-      <c r="D66" s="21"/>
-      <c r="E66" s="21"/>
-      <c r="F66" s="21"/>
-      <c r="G66" s="21"/>
-      <c r="H66" s="21"/>
-      <c r="I66" s="21"/>
-      <c r="J66" s="21"/>
-      <c r="K66" s="21"/>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="10" t="s">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="C69" s="17"/>
+      <c r="D69" s="17"/>
+      <c r="E69" s="17"/>
+      <c r="F69" s="17"/>
+      <c r="G69" s="17"/>
+      <c r="H69" s="17"/>
+      <c r="I69" s="17"/>
+      <c r="J69" s="17"/>
+      <c r="K69" s="17"/>
+      <c r="L69" s="21"/>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C67" s="11" t="s">
+      <c r="C70" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D67" s="11" t="s">
+      <c r="D70" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E67" s="11" t="s">
+      <c r="E70" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F67" s="11" t="s">
+      <c r="F70" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G67" s="11" t="s">
+      <c r="G70" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H67" s="11" t="s">
+      <c r="H70" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I67" s="11" t="s">
+      <c r="I70" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J67" s="11" t="s">
+      <c r="J70" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K67" s="12" t="s">
+      <c r="K70" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="19" t="s">
+      <c r="L70" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C68" s="8" t="s">
+      <c r="C71" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H71" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="I71" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="J71" s="6"/>
+      <c r="K71" s="6"/>
+      <c r="L71" s="21" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="5"/>
+      <c r="C72" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J72" s="6"/>
+      <c r="K72" s="6"/>
+      <c r="L72" s="21"/>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="5"/>
+      <c r="C73" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="J73" s="6"/>
+      <c r="K73" s="6"/>
+      <c r="L73" s="21"/>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="5"/>
+      <c r="C74" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="J74" s="6"/>
+      <c r="K74" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L74" s="21"/>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C77" s="9"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="9"/>
+      <c r="I77" s="9"/>
+      <c r="J77" s="9"/>
+      <c r="K77" s="9"/>
+      <c r="L77" s="4"/>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D78" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E78" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F78" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G78" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H78" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I78" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J78" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K78" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L78" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D68" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="E68" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F68" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G68" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H68" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="I68" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="J68" s="8"/>
-      <c r="K68" s="20"/>
-    </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="19"/>
-      <c r="C69" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="E69" s="8"/>
-      <c r="F69" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G69" s="8"/>
-      <c r="H69" s="8"/>
-      <c r="I69" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="J69" s="8"/>
-      <c r="K69" s="20"/>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="19"/>
-      <c r="C70" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="D70" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="E70" s="8"/>
-      <c r="F70" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G70" s="8"/>
-      <c r="H70" s="8"/>
-      <c r="I70" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="J70" s="8"/>
-      <c r="K70" s="20"/>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="13"/>
-      <c r="C71" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="D71" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="J71" s="14"/>
-      <c r="K71" s="15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="C74" s="9"/>
-      <c r="D74" s="9"/>
-      <c r="E74" s="9"/>
-      <c r="F74" s="9"/>
-      <c r="G74" s="9"/>
-      <c r="H74" s="9"/>
-      <c r="I74" s="9"/>
-      <c r="J74" s="9"/>
-      <c r="K74" s="9"/>
-    </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C75" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D75" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E75" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F75" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G75" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H75" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I75" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="J75" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="K75" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="19" t="s">
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C76" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="D76" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="E76" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F76" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G76" s="8"/>
-      <c r="H76" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="I76" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="J76" s="8"/>
-      <c r="K76" s="20"/>
-    </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="19"/>
-      <c r="C77" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="D77" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="E77" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="F77" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G77" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H77" s="8"/>
-      <c r="I77" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="J77" s="8"/>
-      <c r="K77" s="20"/>
-    </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="19"/>
-      <c r="C78" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="D78" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="E78" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="F78" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G78" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H78" s="8"/>
-      <c r="I78" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="J78" s="8"/>
-      <c r="K78" s="20"/>
-    </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="19"/>
       <c r="C79" s="8" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>176</v>
+        <v>195</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F79" s="8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G79" s="8"/>
-      <c r="H79" s="8"/>
+      <c r="H79" s="8" t="s">
+        <v>196</v>
+      </c>
       <c r="I79" s="8" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="J79" s="8"/>
       <c r="K79" s="20"/>
+      <c r="L79" s="8" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="19" t="s">
-        <v>11</v>
-      </c>
+      <c r="B80" s="19"/>
       <c r="C80" s="8" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="F80" s="8" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H80" s="8" t="s">
-        <v>94</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="H80" s="8"/>
       <c r="I80" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="J80" s="8" t="s">
-        <v>188</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="J80" s="8"/>
       <c r="K80" s="20"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="19"/>
       <c r="C81" s="8" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="F81" s="8" t="s">
         <v>26</v>
       </c>
       <c r="G81" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H81" s="8" t="s">
-        <v>191</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="H81" s="8"/>
       <c r="I81" s="8" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="J81" s="8"/>
       <c r="K81" s="20"/>
@@ -2773,639 +2872,730 @@
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="19"/>
       <c r="C82" s="8" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E82" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F82" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G82" s="8" t="s">
-        <v>53</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G82" s="8"/>
       <c r="H82" s="8"/>
       <c r="I82" s="8" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="J82" s="8"/>
       <c r="K82" s="20"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="13"/>
-      <c r="C83" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="D83" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="E83" s="14"/>
-      <c r="F83" s="14" t="s">
+      <c r="B83" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="E83" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F83" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G83" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H83" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I83" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="J83" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="K83" s="20"/>
+      <c r="L83" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="19"/>
+      <c r="C84" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="E84" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F84" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G84" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H84" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="I84" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="J84" s="8"/>
+      <c r="K84" s="20"/>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B85" s="19"/>
+      <c r="C85" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="E85" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F85" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G85" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H85" s="8"/>
+      <c r="I85" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="J85" s="8"/>
+      <c r="K85" s="20"/>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B86" s="13"/>
+      <c r="C86" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="E86" s="14"/>
+      <c r="F86" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="G83" s="14"/>
-      <c r="H83" s="14"/>
-      <c r="I83" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="J83" s="14"/>
-      <c r="K83" s="15" t="s">
+      <c r="G86" s="14"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="J86" s="14"/>
+      <c r="K86" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="C86" s="9"/>
-      <c r="D86" s="9"/>
-      <c r="E86" s="9"/>
-      <c r="F86" s="9"/>
-      <c r="G86" s="9"/>
-      <c r="H86" s="9"/>
-      <c r="I86" s="9"/>
-      <c r="J86" s="9"/>
-      <c r="K86" s="9"/>
-    </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="10" t="s">
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="C89" s="9"/>
+      <c r="D89" s="9"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="9"/>
+      <c r="G89" s="9"/>
+      <c r="H89" s="9"/>
+      <c r="I89" s="9"/>
+      <c r="J89" s="9"/>
+      <c r="K89" s="9"/>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B90" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C87" s="11" t="s">
+      <c r="C90" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D87" s="11" t="s">
+      <c r="D90" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E87" s="11" t="s">
+      <c r="E90" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F87" s="11" t="s">
+      <c r="F90" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G87" s="11" t="s">
+      <c r="G90" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H87" s="11" t="s">
+      <c r="H90" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I87" s="11" t="s">
+      <c r="I90" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J87" s="11" t="s">
+      <c r="J90" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K87" s="12" t="s">
+      <c r="K90" s="12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="19"/>
-      <c r="C88" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="D88" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="E88" s="8"/>
-      <c r="F88" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G88" s="8"/>
-      <c r="H88" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="I88" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="J88" s="8"/>
-      <c r="K88" s="20"/>
-    </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="19"/>
-      <c r="C89" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="D89" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="E89" s="8"/>
-      <c r="F89" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G89" s="8"/>
-      <c r="H89" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="I89" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="J89" s="8"/>
-      <c r="K89" s="20"/>
-    </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="19"/>
-      <c r="C90" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="D90" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="E90" s="8"/>
-      <c r="F90" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G90" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="H90" s="8"/>
-      <c r="I90" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="J90" s="8"/>
-      <c r="K90" s="20"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="19"/>
       <c r="C91" s="8" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="E91" s="8"/>
       <c r="F91" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G91" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="H91" s="8"/>
+        <v>15</v>
+      </c>
+      <c r="G91" s="8"/>
+      <c r="H91" s="8" t="s">
+        <v>220</v>
+      </c>
       <c r="I91" s="8" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="J91" s="8"/>
       <c r="K91" s="20"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="13"/>
-      <c r="C92" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="D92" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="E92" s="14"/>
-      <c r="F92" s="14" t="s">
+      <c r="B92" s="19"/>
+      <c r="C92" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="D92" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="E92" s="8"/>
+      <c r="F92" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G92" s="8"/>
+      <c r="H92" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="I92" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="J92" s="8"/>
+      <c r="K92" s="20"/>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B93" s="19"/>
+      <c r="C93" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="D93" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="E93" s="8"/>
+      <c r="F93" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G93" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H93" s="8"/>
+      <c r="I93" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="J93" s="8"/>
+      <c r="K93" s="20"/>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B94" s="19"/>
+      <c r="C94" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="E94" s="8"/>
+      <c r="F94" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G94" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="H94" s="8"/>
+      <c r="I94" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="J94" s="8"/>
+      <c r="K94" s="20"/>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B95" s="13"/>
+      <c r="C95" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="D95" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="E95" s="14"/>
+      <c r="F95" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="G92" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="H92" s="14"/>
-      <c r="I92" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="J92" s="14"/>
-      <c r="K92" s="15" t="s">
+      <c r="G95" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="H95" s="14"/>
+      <c r="I95" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="J95" s="14"/>
+      <c r="K95" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="C95" s="9"/>
-      <c r="D95" s="9"/>
-      <c r="E95" s="9"/>
-      <c r="F95" s="9"/>
-      <c r="G95" s="9"/>
-      <c r="H95" s="9"/>
-      <c r="I95" s="9"/>
-      <c r="J95" s="9"/>
-      <c r="K95" s="9"/>
-    </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="10" t="s">
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B98" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="C98" s="9"/>
+      <c r="D98" s="9"/>
+      <c r="E98" s="9"/>
+      <c r="F98" s="9"/>
+      <c r="G98" s="9"/>
+      <c r="H98" s="9"/>
+      <c r="I98" s="9"/>
+      <c r="J98" s="9"/>
+      <c r="K98" s="9"/>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B99" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C96" s="11" t="s">
+      <c r="C99" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D96" s="11" t="s">
+      <c r="D99" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E96" s="11" t="s">
+      <c r="E99" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F96" s="11" t="s">
+      <c r="F99" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G96" s="11" t="s">
+      <c r="G99" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H96" s="11" t="s">
+      <c r="H99" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I96" s="11" t="s">
+      <c r="I99" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J96" s="11" t="s">
+      <c r="J99" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K96" s="12" t="s">
+      <c r="K99" s="12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="D97" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="E97" s="8"/>
-      <c r="F97" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G97" s="8"/>
-      <c r="H97" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="I97" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="J97" s="8"/>
-      <c r="K97" s="20"/>
-    </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="19"/>
-      <c r="C98" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="D98" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="E98" s="8"/>
-      <c r="F98" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G98" s="8"/>
-      <c r="H98" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="I98" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="J98" s="8"/>
-      <c r="K98" s="20"/>
-    </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="19"/>
-      <c r="C99" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="D99" s="8"/>
-      <c r="E99" s="8"/>
-      <c r="F99" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G99" s="8"/>
-      <c r="H99" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I99" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="J99" s="8"/>
-      <c r="K99" s="20"/>
+      <c r="L99" s="0" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B100" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="E100" s="8"/>
       <c r="F100" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G100" s="8" t="s">
-        <v>226</v>
-      </c>
+      <c r="G100" s="8"/>
       <c r="H100" s="8" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="I100" s="8" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="J100" s="8"/>
       <c r="K100" s="20"/>
+      <c r="L100" s="0" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="13"/>
-      <c r="C101" s="14" t="s">
-        <v>229</v>
-      </c>
-      <c r="D101" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="E101" s="14"/>
-      <c r="F101" s="14" t="s">
+      <c r="B101" s="19"/>
+      <c r="C101" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="D101" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="E101" s="8"/>
+      <c r="F101" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G101" s="8"/>
+      <c r="H101" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="I101" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="J101" s="8"/>
+      <c r="K101" s="20"/>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B102" s="19"/>
+      <c r="C102" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="D102" s="8"/>
+      <c r="E102" s="8"/>
+      <c r="F102" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G102" s="8"/>
+      <c r="H102" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I102" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="J102" s="8"/>
+      <c r="K102" s="20"/>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B103" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="D103" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="E103" s="8"/>
+      <c r="F103" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G103" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="H103" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="I103" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="J103" s="8"/>
+      <c r="K103" s="20"/>
+      <c r="L103" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B104" s="13"/>
+      <c r="C104" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="D104" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="E104" s="14"/>
+      <c r="F104" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="G101" s="14"/>
-      <c r="H101" s="14"/>
-      <c r="I101" s="14" t="s">
-        <v>230</v>
-      </c>
-      <c r="J101" s="14"/>
-      <c r="K101" s="15" t="s">
+      <c r="G104" s="14"/>
+      <c r="H104" s="14"/>
+      <c r="I104" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="J104" s="14"/>
+      <c r="K104" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C104" s="9"/>
-      <c r="D104" s="9"/>
-      <c r="E104" s="9"/>
-      <c r="F104" s="9"/>
-      <c r="G104" s="9"/>
-      <c r="H104" s="9"/>
-      <c r="I104" s="9"/>
-      <c r="J104" s="9"/>
-      <c r="K104" s="9"/>
-    </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="10" t="s">
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B107" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C107" s="9"/>
+      <c r="D107" s="9"/>
+      <c r="E107" s="9"/>
+      <c r="F107" s="9"/>
+      <c r="G107" s="9"/>
+      <c r="H107" s="9"/>
+      <c r="I107" s="9"/>
+      <c r="J107" s="9"/>
+      <c r="K107" s="9"/>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B108" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C105" s="11" t="s">
+      <c r="C108" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D105" s="11" t="s">
+      <c r="D108" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E105" s="11" t="s">
+      <c r="E108" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F105" s="11" t="s">
+      <c r="F108" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G105" s="11" t="s">
+      <c r="G108" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H105" s="11" t="s">
+      <c r="H108" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I105" s="11" t="s">
+      <c r="I108" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J105" s="11" t="s">
+      <c r="J108" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K105" s="12" t="s">
+      <c r="K108" s="12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B106" s="19" t="s">
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B109" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C106" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="D106" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="E106" s="8"/>
-      <c r="F106" s="8" t="s">
+      <c r="C109" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="D109" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="E109" s="8"/>
+      <c r="F109" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G106" s="8"/>
-      <c r="H106" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="I106" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="J106" s="8"/>
-      <c r="K106" s="20"/>
-    </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="19" t="s">
+      <c r="G109" s="8"/>
+      <c r="H109" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="I109" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="J109" s="8"/>
+      <c r="K109" s="20"/>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B110" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C107" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="D107" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="E107" s="8"/>
-      <c r="F107" s="8" t="s">
+      <c r="C110" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="D110" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="E110" s="8"/>
+      <c r="F110" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G107" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="H107" s="8"/>
-      <c r="I107" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="J107" s="8"/>
-      <c r="K107" s="20"/>
-    </row>
-    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="19" t="s">
+      <c r="G110" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="H110" s="8"/>
+      <c r="I110" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="J110" s="8"/>
+      <c r="K110" s="20"/>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B111" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C108" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="D108" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="E108" s="8"/>
-      <c r="F108" s="8" t="s">
+      <c r="C111" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="D111" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="E111" s="8"/>
+      <c r="F111" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G108" s="8" t="s">
+      <c r="G111" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="H108" s="8"/>
-      <c r="I108" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="J108" s="8"/>
-      <c r="K108" s="20"/>
-    </row>
-    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B109" s="13" t="s">
+      <c r="H111" s="8"/>
+      <c r="I111" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="J111" s="8"/>
+      <c r="K111" s="20"/>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B112" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C109" s="14" t="s">
-        <v>242</v>
-      </c>
-      <c r="D109" s="14" t="s">
-        <v>243</v>
-      </c>
-      <c r="E109" s="14"/>
-      <c r="F109" s="14" t="s">
+      <c r="C112" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="D112" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="E112" s="14"/>
+      <c r="F112" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G109" s="14"/>
-      <c r="H109" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="I109" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="J109" s="14"/>
-      <c r="K109" s="15"/>
-    </row>
-    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B110" s="7"/>
-      <c r="C110" s="8"/>
-      <c r="D110" s="8"/>
-      <c r="E110" s="8"/>
-      <c r="F110" s="8"/>
-      <c r="G110" s="8"/>
-      <c r="H110" s="8"/>
-      <c r="I110" s="8"/>
-      <c r="J110" s="8"/>
-      <c r="K110" s="8"/>
-    </row>
-    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B111" s="7"/>
-      <c r="C111" s="8"/>
-      <c r="D111" s="8"/>
-      <c r="E111" s="8"/>
-      <c r="F111" s="8"/>
-      <c r="G111" s="8"/>
-      <c r="H111" s="8"/>
-      <c r="I111" s="8"/>
-      <c r="J111" s="8"/>
-      <c r="K111" s="8"/>
-    </row>
-    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B112" s="7"/>
-      <c r="C112" s="8"/>
-      <c r="D112" s="8"/>
-      <c r="E112" s="8"/>
-      <c r="F112" s="8"/>
-      <c r="G112" s="8"/>
-      <c r="H112" s="8"/>
-      <c r="I112" s="8"/>
-      <c r="J112" s="8"/>
-      <c r="K112" s="8"/>
+      <c r="G112" s="14"/>
+      <c r="H112" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="I112" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="J112" s="14"/>
+      <c r="K112" s="15"/>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B113" s="7"/>
+      <c r="C113" s="8"/>
+      <c r="D113" s="8"/>
+      <c r="E113" s="8"/>
+      <c r="F113" s="8"/>
+      <c r="G113" s="8"/>
+      <c r="H113" s="8"/>
+      <c r="I113" s="8"/>
+      <c r="J113" s="8"/>
+      <c r="K113" s="8"/>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B114" s="7"/>
+      <c r="C114" s="8"/>
+      <c r="D114" s="8"/>
+      <c r="E114" s="8"/>
+      <c r="F114" s="8"/>
+      <c r="G114" s="8"/>
+      <c r="H114" s="8"/>
+      <c r="I114" s="8"/>
+      <c r="J114" s="8"/>
+      <c r="K114" s="8"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B115" s="22"/>
-      <c r="C115" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="D115" s="23"/>
-      <c r="E115" s="23"/>
-      <c r="F115" s="23"/>
-      <c r="G115" s="23"/>
-      <c r="H115" s="23"/>
-      <c r="I115" s="23"/>
-      <c r="J115" s="23"/>
-      <c r="K115" s="23"/>
-    </row>
-    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B116" s="10" t="s">
+      <c r="B115" s="7"/>
+      <c r="C115" s="8"/>
+      <c r="D115" s="8"/>
+      <c r="E115" s="8"/>
+      <c r="F115" s="8"/>
+      <c r="G115" s="8"/>
+      <c r="H115" s="8"/>
+      <c r="I115" s="8"/>
+      <c r="J115" s="8"/>
+      <c r="K115" s="8"/>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B118" s="22"/>
+      <c r="C118" s="23" t="s">
+        <v>265</v>
+      </c>
+      <c r="D118" s="23"/>
+      <c r="E118" s="23"/>
+      <c r="F118" s="23"/>
+      <c r="G118" s="23"/>
+      <c r="H118" s="23"/>
+      <c r="I118" s="23"/>
+      <c r="J118" s="23"/>
+      <c r="K118" s="23"/>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B119" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C116" s="11" t="s">
+      <c r="C119" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D116" s="11" t="s">
+      <c r="D119" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E116" s="11" t="s">
+      <c r="E119" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F116" s="11" t="s">
+      <c r="F119" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G116" s="11" t="s">
+      <c r="G119" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H116" s="11" t="s">
+      <c r="H119" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I116" s="11" t="s">
+      <c r="I119" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J116" s="11" t="s">
+      <c r="J119" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K116" s="12" t="s">
+      <c r="K119" s="12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B117" s="13"/>
-      <c r="C117" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="D117" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="E117" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="F117" s="14" t="s">
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B120" s="13"/>
+      <c r="C120" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="D120" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="E120" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="F120" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G117" s="14"/>
-      <c r="H117" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="I117" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="J117" s="14"/>
-      <c r="K117" s="15"/>
-    </row>
-    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B118" s="7"/>
-      <c r="C118" s="8"/>
-      <c r="D118" s="8"/>
-      <c r="E118" s="8"/>
-      <c r="F118" s="8"/>
-      <c r="G118" s="8"/>
-      <c r="H118" s="8"/>
-      <c r="I118" s="8"/>
-      <c r="J118" s="8"/>
-      <c r="K118" s="8"/>
-    </row>
-    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B119" s="7"/>
-      <c r="C119" s="8"/>
-      <c r="D119" s="8"/>
-      <c r="E119" s="8"/>
-      <c r="F119" s="8"/>
-      <c r="G119" s="8"/>
-      <c r="H119" s="8"/>
-      <c r="I119" s="8"/>
-      <c r="J119" s="8"/>
-      <c r="K119" s="8"/>
-    </row>
+      <c r="G120" s="14"/>
+      <c r="H120" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="I120" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="J120" s="14"/>
+      <c r="K120" s="15"/>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B121" s="7"/>
+      <c r="C121" s="8"/>
+      <c r="D121" s="8"/>
+      <c r="E121" s="8"/>
+      <c r="F121" s="8"/>
+      <c r="G121" s="8"/>
+      <c r="H121" s="8"/>
+      <c r="I121" s="8"/>
+      <c r="J121" s="8"/>
+      <c r="K121" s="8"/>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B122" s="7"/>
+      <c r="C122" s="8"/>
+      <c r="D122" s="8"/>
+      <c r="E122" s="8"/>
+      <c r="F122" s="8"/>
+      <c r="G122" s="8"/>
+      <c r="H122" s="8"/>
+      <c r="I122" s="8"/>
+      <c r="J122" s="8"/>
+      <c r="K122" s="8"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="C2:K2"/>
@@ -3413,13 +3603,13 @@
     <mergeCell ref="B24:K24"/>
     <mergeCell ref="B36:K36"/>
     <mergeCell ref="B45:K45"/>
-    <mergeCell ref="B57:K57"/>
-    <mergeCell ref="B66:K66"/>
-    <mergeCell ref="B74:K74"/>
-    <mergeCell ref="B86:K86"/>
-    <mergeCell ref="B95:K95"/>
-    <mergeCell ref="B104:K104"/>
-    <mergeCell ref="C115:K115"/>
+    <mergeCell ref="B60:K60"/>
+    <mergeCell ref="B69:K69"/>
+    <mergeCell ref="B77:K77"/>
+    <mergeCell ref="B89:K89"/>
+    <mergeCell ref="B98:K98"/>
+    <mergeCell ref="B107:K107"/>
+    <mergeCell ref="C118:K118"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3438,7 +3628,7 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added bind parents function
</commit_message>
<xml_diff>
--- a/API List.xlsx
+++ b/API List.xlsx
@@ -236,7 +236,7 @@
     <t xml:space="preserve">/api/v1.0/bind_parents</t>
   </si>
   <si>
-    <t xml:space="preserve">student_id, relation</t>
+    <t xml:space="preserve">teacher_id, student_id, relation, phone, real_name, nick_name, gender, language, province, city, avatar, roles</t>
   </si>
   <si>
     <t xml:space="preserve">Bind a parent with a student</t>
@@ -1109,8 +1109,8 @@
   </sheetPr>
   <dimension ref="B1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B91" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B14" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>